<commit_message>
picker updated with default value
</commit_message>
<xml_diff>
--- a/PTA/platforms/browser/www/testBank.xlsx
+++ b/PTA/platforms/browser/www/testBank.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prototype\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calvin\Documents\PTAlso\PTA\PTA\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="406">
   <si>
     <t>Which of the following is NOT a type of motherboard expansion slot?</t>
   </si>
@@ -477,13 +477,801 @@
   </si>
   <si>
     <t xml:space="preserve">Light Emitting Diode(LED) or Liquid Crystal Displays (LCD) screens are much better at displacing glare than the other technolgy combinations. </t>
+  </si>
+  <si>
+    <r>
+      <t>the main functionality of the basic input/output system (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BIOS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) is to perform the initial hardware checks after the computer is powered on and start up the OS</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">true </t>
+  </si>
+  <si>
+    <t>in modern PCs, the procedure of replacing BIOS contents is sometimes refered to as:</t>
+  </si>
+  <si>
+    <t>hard boot</t>
+  </si>
+  <si>
+    <t>overclock</t>
+  </si>
+  <si>
+    <t>flashing the BIOS</t>
+  </si>
+  <si>
+    <t>Direct memory access DMA</t>
+  </si>
+  <si>
+    <t>Flashing the BIOS</t>
+  </si>
+  <si>
+    <t>A+S</t>
+  </si>
+  <si>
+    <t>which Microsoft Windows OS utility can be used to view basic information about computers BIOS</t>
+  </si>
+  <si>
+    <t>WINVER&gt;EXE</t>
+  </si>
+  <si>
+    <t>MSINFO32.EXE</t>
+  </si>
+  <si>
+    <t>controle panel</t>
+  </si>
+  <si>
+    <t>SERVICES.MSC</t>
+  </si>
+  <si>
+    <t>power failure during BIOS upgrade can be the cause of irreversible damage to the computer system</t>
+  </si>
+  <si>
+    <t>after normal system shutdown, when the computer is turned off, contents of the memory used to store BIOS setting are:</t>
+  </si>
+  <si>
+    <t>Erased</t>
+  </si>
+  <si>
+    <t>Retained</t>
+  </si>
+  <si>
+    <t>Stored in a page file</t>
+  </si>
+  <si>
+    <t>Saved on a harddrive</t>
+  </si>
+  <si>
+    <t>Rettained</t>
+  </si>
+  <si>
+    <t>which of the acronyms listed below refers to a series of basic hardware diagnostic test performed by the BIOS after the computer is powered on?</t>
+  </si>
+  <si>
+    <t>IDE</t>
+  </si>
+  <si>
+    <t>Qos</t>
+  </si>
+  <si>
+    <t>after completing the initial diagnostics and assigning system resources, the startup Bios program checks for information about secondary storage devices that might contain the OS.  The list of devices and the order in which they should be checked can be found and arranged in th CMOS setu utility, and this option is commonly refered to as:</t>
+  </si>
+  <si>
+    <t>boot record</t>
+  </si>
+  <si>
+    <t>Master Boot Record(MBR)</t>
+  </si>
+  <si>
+    <t>Partition table</t>
+  </si>
+  <si>
+    <t>Bootsequence</t>
+  </si>
+  <si>
+    <t>Boot sequence</t>
+  </si>
+  <si>
+    <t>in order to work, an integrated component such as Network Interface Card(NIC) on a newly assembled computer system may need to be first</t>
+  </si>
+  <si>
+    <t>Enabled in Windows Controle Panel</t>
+  </si>
+  <si>
+    <t>Updated with the latest driver in Device Manager</t>
+  </si>
+  <si>
+    <t>Checked against the Hardware Compatibility List (HCL)</t>
+  </si>
+  <si>
+    <t>Enabled in the advances BIOS settings menu</t>
+  </si>
+  <si>
+    <t>Enabled in the advanced BIOS settings menu</t>
+  </si>
+  <si>
+    <t>After launching Windows Virtual PC application technician recives error message stating that the Hardware-Assisted Virtualization(HAV) feature is not enabled on the computer. Which of the folowing steps might help in fixing this problem?</t>
+  </si>
+  <si>
+    <t>increasing the amount of phisical RAM on the system</t>
+  </si>
+  <si>
+    <t>Re-instlling Windows Virtual PC app</t>
+  </si>
+  <si>
+    <t xml:space="preserve">getting into the CMOS setup utility and enabling the virtualization technology setting </t>
+  </si>
+  <si>
+    <t>Safe Mode troubleshooting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Getting the CMOS setup utility and Enabling the virtualization technology setting </t>
+  </si>
+  <si>
+    <t>the CMOS setup utility can be accessed by pressing:</t>
+  </si>
+  <si>
+    <t>Reset button on the front panel of the computer case</t>
+  </si>
+  <si>
+    <t>the key set by the motherboard manufacturer for accessing CMOS setup utility during boot</t>
+  </si>
+  <si>
+    <t>Del key during boot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1 key while loged into Windows </t>
+  </si>
+  <si>
+    <t>Which of the folowing answers refers to a firmware interface designed as a replacement for BIOS?</t>
+  </si>
+  <si>
+    <t>UEFI</t>
+  </si>
+  <si>
+    <t>CMOS</t>
+  </si>
+  <si>
+    <t>USMT</t>
+  </si>
+  <si>
+    <t>Which of the folowing statements is true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aborted BIOS update can be resumed by the transaction recovery system </t>
+  </si>
+  <si>
+    <t>a common securtiy measure is to store BIOS on a non-rewriteable memory chip</t>
+  </si>
+  <si>
+    <t>the process of BIOS update can be aborted and resumed at a later time</t>
+  </si>
+  <si>
+    <t>Aborted BIOS update could render the computer unusable</t>
+  </si>
+  <si>
+    <t>aborted BIOS update could render the computer unusable</t>
+  </si>
+  <si>
+    <t>which type of password provides the hightst level of permissions in BIOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">root </t>
+  </si>
+  <si>
+    <t>supervisor</t>
+  </si>
+  <si>
+    <t>administrator</t>
+  </si>
+  <si>
+    <t>power user</t>
+  </si>
+  <si>
+    <t>what is LoJack?</t>
+  </si>
+  <si>
+    <t>loopback adapter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secutity feature used for locating stolen desktops, laptops, or tablets </t>
+  </si>
+  <si>
+    <t>Conector standard</t>
+  </si>
+  <si>
+    <t>RJ_11 plug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Security feature used for locating stolen Desktops, laptops, or tablets </t>
+  </si>
+  <si>
+    <t>which of the folowing terms refer to a tech that allows for storing passwords, certificates, or encryption keys in a hardware chip?</t>
+  </si>
+  <si>
+    <t>Access Controle List (ACL)</t>
+  </si>
+  <si>
+    <t>Encrypting File System(EFS)</t>
+  </si>
+  <si>
+    <t>User Account Controle (UAC)</t>
+  </si>
+  <si>
+    <t>Trusted Platform Module (TPM)</t>
+  </si>
+  <si>
+    <t>Trusted Platform Module(TPM)</t>
+  </si>
+  <si>
+    <t>while tryign to enable the entire drive encryption feature in windows technician receives the followling error message: "A compatible Trusted Platform Module(TPM) security Device must be present on this computer, but a TPM was not found." knowing that the system had a TPM chip installed, which of the folowing steps might help in solving this problem?</t>
+  </si>
+  <si>
+    <t>Re-install OS</t>
+  </si>
+  <si>
+    <t>Enableing the TPM security feture in CMOS setup menu</t>
+  </si>
+  <si>
+    <t>Hard drive replacement</t>
+  </si>
+  <si>
+    <t>Enabling the TPM security feature in Windows controle panel</t>
+  </si>
+  <si>
+    <t>Enabling the TPM security in CMOS setup menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A computer supporting LoJack tech has two main componets installed: a Application Agent residing in he os which sends tracking signals to the monitoring center allowing the law enforcement to locate and recover stolen device, andd Persistence Module  which restores the Application Agent and allows it to survive os re-installation or hard drive format: the highest level of security offered by LoJack can be achieved when Persistence Module resides in </t>
+  </si>
+  <si>
+    <t>os</t>
+  </si>
+  <si>
+    <t>Partition gap on hard drive</t>
+  </si>
+  <si>
+    <t>Computers BIOS</t>
+  </si>
+  <si>
+    <t>USB key</t>
+  </si>
+  <si>
+    <t>A UEFI functionality designed to prevent the loading of malware and unauthorized Oss during system start-up is known as:</t>
+  </si>
+  <si>
+    <t>LoJack</t>
+  </si>
+  <si>
+    <t>Bitlocker</t>
+  </si>
+  <si>
+    <t>Secure boot</t>
+  </si>
+  <si>
+    <t>Kerberos</t>
+  </si>
+  <si>
+    <t>Similarly to magnetic drives, Solid State-Drives (SSD) require periodic defragmentation in order to improve system performance.</t>
+  </si>
+  <si>
+    <t>a tiny sopt on the LCD monitor display screen that permanetly remains black when it should be activated and displaying color is commonly refered to as stuck pixel.</t>
+  </si>
+  <si>
+    <t>a permanent computer display screen discoloration caused by displaying the same static image for extended periods of time is known as:</t>
+  </si>
+  <si>
+    <t>Artifact</t>
+  </si>
+  <si>
+    <t>Stuck pixel</t>
+  </si>
+  <si>
+    <t>Burn-in</t>
+  </si>
+  <si>
+    <t>Dead pixel</t>
+  </si>
+  <si>
+    <t>which of the folowing command-line utilities allows to test the reachability of a host across an IP network</t>
+  </si>
+  <si>
+    <t>NETSTAT</t>
+  </si>
+  <si>
+    <t>IPCONFIG</t>
+  </si>
+  <si>
+    <t>TRACERT</t>
+  </si>
+  <si>
+    <t>PING</t>
+  </si>
+  <si>
+    <t>NET CONFIG</t>
+  </si>
+  <si>
+    <t>IFCONFIG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">which of the folowing command-line prompt tools listed below allows to display IP addresses, subnet mask, and default gateway for all adaptors? </t>
+  </si>
+  <si>
+    <t>A Linux comand-line utility used for displaying and modifying network interface configuration settings is called</t>
+  </si>
+  <si>
+    <t>NETWORKSETUP</t>
+  </si>
+  <si>
+    <t>Microsoft Windows OS command-line for displaying intermediary points on the packet route is called</t>
+  </si>
+  <si>
+    <t>ROUTE PRINT</t>
+  </si>
+  <si>
+    <t>TRACEOUTE</t>
+  </si>
+  <si>
+    <t>N+</t>
+  </si>
+  <si>
+    <t>which of the folowing is an example of active eavesdropping</t>
+  </si>
+  <si>
+    <t>Phishing</t>
+  </si>
+  <si>
+    <t>DDoS</t>
+  </si>
+  <si>
+    <t>Xmas attack</t>
+  </si>
+  <si>
+    <t>MITM</t>
+  </si>
+  <si>
+    <t>Switch spoofing and double tagging are two primary methods of attacking networked resources on:</t>
+  </si>
+  <si>
+    <t>WLAN</t>
+  </si>
+  <si>
+    <t>VLAN</t>
+  </si>
+  <si>
+    <t>VPN</t>
+  </si>
+  <si>
+    <t>PAN</t>
+  </si>
+  <si>
+    <t>Harmful programs used to disrupt computer operation, gather sensitive information, or gain access to private computer systems are commonly referred to as:</t>
+  </si>
+  <si>
+    <t>Malware</t>
+  </si>
+  <si>
+    <t>Adware</t>
+  </si>
+  <si>
+    <t>Spyware</t>
+  </si>
+  <si>
+    <t>Computer viruses</t>
+  </si>
+  <si>
+    <t>Zero-day attack exploits:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New accounts </t>
+  </si>
+  <si>
+    <t>Packed software</t>
+  </si>
+  <si>
+    <t>well known vulberability</t>
+  </si>
+  <si>
+    <t>Vulnerability that is present in already released software but unknown to the software developer</t>
+  </si>
+  <si>
+    <t>one of the measures for securing network devices includes the practice of disabling unsused ports.</t>
+  </si>
+  <si>
+    <t>a hacker has captured network traffic with cleartext commands sent from the client to the server console. Which of the following ports is being used by the network admin for the client-server communication?</t>
+  </si>
+  <si>
+    <t>which of the folowing answers refers to preferred replacement for SLIP protocol</t>
+  </si>
+  <si>
+    <t>PPP</t>
+  </si>
+  <si>
+    <t>PoE</t>
+  </si>
+  <si>
+    <t>CHAP</t>
+  </si>
+  <si>
+    <t>PAP</t>
+  </si>
+  <si>
+    <t>FTPS is an extension to the Secure Shell Protocol (SSH) and runs by default on port number 22</t>
+  </si>
+  <si>
+    <t>which of the following protocols does not provide authentication?</t>
+  </si>
+  <si>
+    <t>FTP</t>
+  </si>
+  <si>
+    <t>SCP</t>
+  </si>
+  <si>
+    <t>TFTP</t>
+  </si>
+  <si>
+    <t>SFTP</t>
+  </si>
+  <si>
+    <t>of the three exsiting versions of the Simple Network Management Protocol (SNMP) versions 1 and 2 (SNMPv1 and SNMPv2) offer authentication based on community strings sent in an unencrypted form (in cleartext). SNMPv3 provides packet encryption, authentication, and hasning mechanisms that allow for checking whether data has changed in transit.</t>
+  </si>
+  <si>
+    <t>which of the following answers refers to a cryptographic network protocol for secure data communication, remote command-line login, remote command execution, and other secure network services between computers?</t>
+  </si>
+  <si>
+    <t>Telnet</t>
+  </si>
+  <si>
+    <t>SSH</t>
+  </si>
+  <si>
+    <t>Bcrypt</t>
+  </si>
+  <si>
+    <t>which of the protocols listed below was designed as a secure replacement for Telnet</t>
+  </si>
+  <si>
+    <t>LDAP</t>
+  </si>
+  <si>
+    <t>the SCP protocol is used for:</t>
+  </si>
+  <si>
+    <t>Directory access</t>
+  </si>
+  <si>
+    <t>Secure file transfer</t>
+  </si>
+  <si>
+    <t>Network addressing</t>
+  </si>
+  <si>
+    <t>Sending emails</t>
+  </si>
+  <si>
+    <t>Which ot the Ipsec modes provides entire packet encryption?</t>
+  </si>
+  <si>
+    <t>Tunnel</t>
+  </si>
+  <si>
+    <t>Payload</t>
+  </si>
+  <si>
+    <t>Transport</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>which of the following solutions provides a shielded environment that protects against unintentional signal leakage and eavesdropping</t>
+  </si>
+  <si>
+    <t>SCADA</t>
+  </si>
+  <si>
+    <t>TEMPEST</t>
+  </si>
+  <si>
+    <t>HVAC</t>
+  </si>
+  <si>
+    <t>RADIUS</t>
+  </si>
+  <si>
+    <t>Data files containing detection and remediation code that antivirus or antispyware products use to identify malicious code are known as</t>
+  </si>
+  <si>
+    <t>Repositories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">signature files </t>
+  </si>
+  <si>
+    <t>macros</t>
+  </si>
+  <si>
+    <t>Security logs</t>
+  </si>
+  <si>
+    <t>signature files</t>
+  </si>
+  <si>
+    <t>the term "DHCP snooping" refers to an exploit that enables operation of a rouge DHCP server on a network.</t>
+  </si>
+  <si>
+    <t>Simple Mail Transfer Protocol(SMTP) operates with the use of TCP port:</t>
+  </si>
+  <si>
+    <t>Which of the potr numbers listed below is commonly used for Session Iniation Protocol (SIP) non-encrypted traffic?</t>
+  </si>
+  <si>
+    <t>Port number 5061 is typically used for Session Initiation Protocol (SIP) traffic encrypted with Transport Layre Security (TLS)</t>
+  </si>
+  <si>
+    <t>port number 5004 is used by:</t>
+  </si>
+  <si>
+    <t>MGCP</t>
+  </si>
+  <si>
+    <t>RTP</t>
+  </si>
+  <si>
+    <t>H.323</t>
+  </si>
+  <si>
+    <t>RTCP</t>
+  </si>
+  <si>
+    <t>RTP contorl Protocol RTCP runs by defalt on port</t>
+  </si>
+  <si>
+    <t>TCP port 1720 is the default port number for</t>
+  </si>
+  <si>
+    <t>PPTP</t>
+  </si>
+  <si>
+    <t>User Datagram Protocol (UDP) is a connection- oriented protocol that requires a set of initial steps in order to establish a connection, supports retransmission of lost packets, flow control, or sequencing</t>
+  </si>
+  <si>
+    <t>Transmission Controle Protocol(tcp) is an example of connectionless protocol. TCP doesn’t support three-way handshake</t>
+  </si>
+  <si>
+    <t>Which of the following protocols is used in network management systems for monitoring network- attached devices?</t>
+  </si>
+  <si>
+    <t>IMAP</t>
+  </si>
+  <si>
+    <t>SNMP</t>
+  </si>
+  <si>
+    <t>An SNMP Agent recives request on UDP port:</t>
+  </si>
+  <si>
+    <t>Which of the following answers lists a cryptographic network protocol for secure data communication, remote command-line login, remote command execution, and other secure network services between two networked computers?</t>
+  </si>
+  <si>
+    <t>A hacker has captured network traffic with cleartext commands sent from the client to the server console. Which of the following ports is being used by the network admin for the client-server communication?</t>
+  </si>
+  <si>
+    <t>A network administrator wants to replace a service running on port 23 with a more reliable solution. Which of the following ports would be in use after implementing this change?</t>
+  </si>
+  <si>
+    <t>DNS runs on port:</t>
+  </si>
+  <si>
+    <t>UDP port 67 is used by:</t>
+  </si>
+  <si>
+    <t>Bootstrap Protocol(BOOTP)</t>
+  </si>
+  <si>
+    <t>remote authentication Dial in user service (RADIUS)</t>
+  </si>
+  <si>
+    <t>Simple Network Management Protocol SNMP</t>
+  </si>
+  <si>
+    <t>Merberos</t>
+  </si>
+  <si>
+    <t>which of the file transfer protocols listed below runs on port number 69 and does not provide authentication?</t>
+  </si>
+  <si>
+    <t>TCP port 445 is used by:</t>
+  </si>
+  <si>
+    <t>RDP</t>
+  </si>
+  <si>
+    <t>SMB</t>
+  </si>
+  <si>
+    <t>SIP</t>
+  </si>
+  <si>
+    <t>A network technician uses an RDP client on their Windows OS in order to remotely troubleshoot a problem on another Windows machine. Which of the following ports needs to be opened for the built-in Windows RDP server to allow this type of network connection?</t>
+  </si>
+  <si>
+    <t>A double colon in an IPv6 address indicates that part of the address containing only zeroes has been compressed to make the address shorter</t>
+  </si>
+  <si>
+    <t>Which of the following answers lists a valid address of FE80:0000:0000:0000:02AA:0000:4C00:FE9A after compression?</t>
+  </si>
+  <si>
+    <t>FE80::2AA::4C00:FE9A</t>
+  </si>
+  <si>
+    <t>FE80:0:2AA:0:4C:FE9A</t>
+  </si>
+  <si>
+    <t>FE80:0:02AA::4C:FE9A</t>
+  </si>
+  <si>
+    <t>An IPv4 to IPv6 transition mechanism that allows IPv6 packets to be transmitted over an IPv4 network is known as:</t>
+  </si>
+  <si>
+    <t>6to4</t>
+  </si>
+  <si>
+    <t>802.3af</t>
+  </si>
+  <si>
+    <t>eDiscovery</t>
+  </si>
+  <si>
+    <t>Miredo</t>
+  </si>
+  <si>
+    <t>What does the term "Miredo" refer to?</t>
+  </si>
+  <si>
+    <t>IPv4 to IPV6 migration mechanism</t>
+  </si>
+  <si>
+    <t>Load balancing solution</t>
+  </si>
+  <si>
+    <t>TeredoIPv6</t>
+  </si>
+  <si>
+    <t>Content filtering solution</t>
+  </si>
+  <si>
+    <t>Teredo IPv6 tunneling software</t>
+  </si>
+  <si>
+    <t>Which of the following answers lists the binary notation of the decimal number 192?</t>
+  </si>
+  <si>
+    <t>an Ipv 4 address consists of:</t>
+  </si>
+  <si>
+    <t>32bits</t>
+  </si>
+  <si>
+    <t>48bits</t>
+  </si>
+  <si>
+    <t>64bits</t>
+  </si>
+  <si>
+    <t>128bits</t>
+  </si>
+  <si>
+    <t>Which of the following is an example of a valid subnet mask?</t>
+  </si>
+  <si>
+    <t>255.255.225.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None of the above is a valid subnet mask </t>
+  </si>
+  <si>
+    <t>255.255.191.0</t>
+  </si>
+  <si>
+    <t>255.255.64.0</t>
+  </si>
+  <si>
+    <t>Which of the following answers lists the default (classful) subnet mask for a class A network?</t>
+  </si>
+  <si>
+    <t>192.168.0.3</t>
+  </si>
+  <si>
+    <t>169.254.10.20</t>
+  </si>
+  <si>
+    <t>65.55.57.27</t>
+  </si>
+  <si>
+    <t>255.0.0.0</t>
+  </si>
+  <si>
+    <t>255.128.0.0</t>
+  </si>
+  <si>
+    <t>224.0.0.0</t>
+  </si>
+  <si>
+    <t>255.244.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 127.0.0.1 </t>
+  </si>
+  <si>
+    <t>APIPA-assigned addresses are valid only for communications within a network segment that a given host is connected to (a host with APIPA-assigned address cannot connect to the Internet).</t>
+  </si>
+  <si>
+    <t>Which of the following answers lists the default (classful) subnet mask for a class C network?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">255.255.192.0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">255.255.224.0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">255.255.252.0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> An IPv4 address in the range 169.254.1.0 through 169.254.254.255 indicates a problem with what type of service?</t>
+  </si>
+  <si>
+    <t>In IPv4 addressing, the leading octet of an IP address with a value of 1 through 126 denotes that the IP address within that range belongs to the:</t>
+  </si>
+  <si>
+    <t>Class A address space</t>
+  </si>
+  <si>
+    <t>Class B address space</t>
+  </si>
+  <si>
+    <t>Class D address space</t>
+  </si>
+  <si>
+    <t>In IPv4 addressing, the leading octet of an IP address with a value of 192 through 223 denotes that the IP address within that range belongs to the:</t>
+  </si>
+  <si>
+    <t>Class C Address space</t>
+  </si>
+  <si>
+    <t>Class C address space</t>
+  </si>
+  <si>
+    <t>I'm sure you know why (Placeholder)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -492,6 +1280,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF333333"/>
       <name val="Calibri"/>
@@ -837,10 +1633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="G105" sqref="G105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1501,68 +2297,1872 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C26" t="b">
+        <v>0</v>
+      </c>
+      <c r="F26" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H26" t="s">
-        <v>6</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H27" t="s">
-        <v>6</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H28" t="s">
-        <v>6</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C29" t="b">
+        <v>0</v>
+      </c>
+      <c r="F29" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H29" t="s">
-        <v>6</v>
+        <v>159</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H30" t="s">
-        <v>6</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H31" t="s">
-        <v>6</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H32" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="8:8" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="8:8" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="8:8" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="8:8" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H36" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="8:8" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H37" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="8:8" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H38" t="s">
-        <v>6</v>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C44" t="b">
+        <v>0</v>
+      </c>
+      <c r="F44" t="b">
+        <v>0</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C45" t="b">
+        <v>0</v>
+      </c>
+      <c r="F45" t="b">
+        <v>0</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H53" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F54" t="s">
+        <v>281</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H54" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F55" t="b">
+        <v>1</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H55" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B56">
+        <v>49</v>
+      </c>
+      <c r="C56">
+        <v>23</v>
+      </c>
+      <c r="D56">
+        <v>68</v>
+      </c>
+      <c r="E56">
+        <v>22</v>
+      </c>
+      <c r="F56">
+        <v>23</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H56" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H57" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C58" t="b">
+        <v>0</v>
+      </c>
+      <c r="F58" t="b">
+        <v>1</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H58" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C59" t="s">
+        <v>292</v>
+      </c>
+      <c r="D59" t="s">
+        <v>293</v>
+      </c>
+      <c r="E59" t="s">
+        <v>294</v>
+      </c>
+      <c r="F59" t="s">
+        <v>293</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H59" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C60" t="b">
+        <v>0</v>
+      </c>
+      <c r="F60" t="b">
+        <v>1</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H60" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C61" t="s">
+        <v>298</v>
+      </c>
+      <c r="D61" t="s">
+        <v>299</v>
+      </c>
+      <c r="E61" t="s">
+        <v>293</v>
+      </c>
+      <c r="F61" t="s">
+        <v>298</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H61" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C62" t="s">
+        <v>301</v>
+      </c>
+      <c r="D62" t="s">
+        <v>291</v>
+      </c>
+      <c r="E62" t="s">
+        <v>287</v>
+      </c>
+      <c r="F62" t="s">
+        <v>298</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H62" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C63" t="s">
+        <v>304</v>
+      </c>
+      <c r="D63" t="s">
+        <v>305</v>
+      </c>
+      <c r="E63" t="s">
+        <v>306</v>
+      </c>
+      <c r="F63" t="s">
+        <v>304</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H63" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C64" t="s">
+        <v>309</v>
+      </c>
+      <c r="D64" t="s">
+        <v>310</v>
+      </c>
+      <c r="E64" t="s">
+        <v>311</v>
+      </c>
+      <c r="F64" t="s">
+        <v>308</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H64" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C65" t="s">
+        <v>313</v>
+      </c>
+      <c r="D65" t="s">
+        <v>315</v>
+      </c>
+      <c r="E65" t="s">
+        <v>316</v>
+      </c>
+      <c r="F65" t="s">
+        <v>314</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H65" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C66" t="s">
+        <v>319</v>
+      </c>
+      <c r="D66" t="s">
+        <v>320</v>
+      </c>
+      <c r="E66" t="s">
+        <v>321</v>
+      </c>
+      <c r="F66" t="s">
+        <v>322</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H66" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C67" t="b">
+        <v>0</v>
+      </c>
+      <c r="F67" t="b">
+        <v>0</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H67" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B68">
+        <v>110</v>
+      </c>
+      <c r="C68">
+        <v>23</v>
+      </c>
+      <c r="D68">
+        <v>143</v>
+      </c>
+      <c r="E68">
+        <v>25</v>
+      </c>
+      <c r="F68">
+        <v>25</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H68" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B69">
+        <v>5004</v>
+      </c>
+      <c r="C69">
+        <v>5005</v>
+      </c>
+      <c r="D69">
+        <v>5060</v>
+      </c>
+      <c r="E69">
+        <v>5061</v>
+      </c>
+      <c r="F69">
+        <v>5060</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H69" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C70" t="b">
+        <v>0</v>
+      </c>
+      <c r="F70" t="b">
+        <v>0</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H70" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C71" t="s">
+        <v>329</v>
+      </c>
+      <c r="D71" t="s">
+        <v>330</v>
+      </c>
+      <c r="E71" t="s">
+        <v>331</v>
+      </c>
+      <c r="F71" t="s">
+        <v>329</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H71" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B72">
+        <v>5004</v>
+      </c>
+      <c r="C72">
+        <v>5060</v>
+      </c>
+      <c r="D72">
+        <v>5005</v>
+      </c>
+      <c r="E72">
+        <v>5061</v>
+      </c>
+      <c r="F72">
+        <v>5005</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H72" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B73" t="s">
+        <v>328</v>
+      </c>
+      <c r="C73" t="s">
+        <v>330</v>
+      </c>
+      <c r="D73" t="s">
+        <v>334</v>
+      </c>
+      <c r="E73" t="s">
+        <v>329</v>
+      </c>
+      <c r="F73" t="s">
+        <v>330</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H73" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B74" t="s">
+        <v>152</v>
+      </c>
+      <c r="C74" t="b">
+        <v>0</v>
+      </c>
+      <c r="F74" t="b">
+        <v>0</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H74" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B75" t="s">
+        <v>152</v>
+      </c>
+      <c r="C75" t="b">
+        <v>0</v>
+      </c>
+      <c r="F75" t="b">
+        <v>0</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H75" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B76" t="s">
+        <v>329</v>
+      </c>
+      <c r="C76" t="s">
+        <v>338</v>
+      </c>
+      <c r="D76" t="s">
+        <v>339</v>
+      </c>
+      <c r="E76" t="s">
+        <v>331</v>
+      </c>
+      <c r="F76" t="s">
+        <v>339</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H76" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B77">
+        <v>161</v>
+      </c>
+      <c r="C77">
+        <v>138</v>
+      </c>
+      <c r="D77">
+        <v>162</v>
+      </c>
+      <c r="E77">
+        <v>139</v>
+      </c>
+      <c r="F77">
+        <v>161</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H77" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B78" t="s">
+        <v>297</v>
+      </c>
+      <c r="C78" t="s">
+        <v>298</v>
+      </c>
+      <c r="D78" t="s">
+        <v>299</v>
+      </c>
+      <c r="E78" t="s">
+        <v>293</v>
+      </c>
+      <c r="F78" t="s">
+        <v>298</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H78" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>342</v>
+      </c>
+      <c r="B79">
+        <v>49</v>
+      </c>
+      <c r="C79">
+        <v>23</v>
+      </c>
+      <c r="D79">
+        <v>68</v>
+      </c>
+      <c r="E79">
+        <v>22</v>
+      </c>
+      <c r="F79">
+        <v>23</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H79" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>343</v>
+      </c>
+      <c r="B80">
+        <v>20</v>
+      </c>
+      <c r="C80">
+        <v>21</v>
+      </c>
+      <c r="D80">
+        <v>22</v>
+      </c>
+      <c r="E80">
+        <v>25</v>
+      </c>
+      <c r="F80">
+        <v>22</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H80" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B81">
+        <v>139</v>
+      </c>
+      <c r="C81">
+        <v>53</v>
+      </c>
+      <c r="D81">
+        <v>443</v>
+      </c>
+      <c r="E81">
+        <v>22</v>
+      </c>
+      <c r="F81">
+        <v>53</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H81" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B82" t="s">
+        <v>346</v>
+      </c>
+      <c r="C82" t="s">
+        <v>347</v>
+      </c>
+      <c r="D82" t="s">
+        <v>348</v>
+      </c>
+      <c r="E82" t="s">
+        <v>349</v>
+      </c>
+      <c r="F82" t="s">
+        <v>346</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H82" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B83" t="s">
+        <v>291</v>
+      </c>
+      <c r="C83" t="s">
+        <v>293</v>
+      </c>
+      <c r="D83" t="s">
+        <v>292</v>
+      </c>
+      <c r="E83" t="s">
+        <v>294</v>
+      </c>
+      <c r="F83" t="s">
+        <v>293</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H83" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B84" t="s">
+        <v>352</v>
+      </c>
+      <c r="C84" t="s">
+        <v>353</v>
+      </c>
+      <c r="D84" t="s">
+        <v>354</v>
+      </c>
+      <c r="E84" t="s">
+        <v>329</v>
+      </c>
+      <c r="F84" t="s">
+        <v>353</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H84" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>355</v>
+      </c>
+      <c r="B85">
+        <v>1701</v>
+      </c>
+      <c r="C85">
+        <v>139</v>
+      </c>
+      <c r="D85">
+        <v>3389</v>
+      </c>
+      <c r="E85">
+        <v>110</v>
+      </c>
+      <c r="F85">
+        <v>3389</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H85" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>356</v>
+      </c>
+      <c r="B86" t="s">
+        <v>152</v>
+      </c>
+      <c r="C86" t="b">
+        <v>0</v>
+      </c>
+      <c r="F86" t="b">
+        <v>1</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H86" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>357</v>
+      </c>
+      <c r="B87" t="s">
+        <v>358</v>
+      </c>
+      <c r="C87" t="s">
+        <v>359</v>
+      </c>
+      <c r="D87" t="s">
+        <v>359</v>
+      </c>
+      <c r="E87" t="s">
+        <v>360</v>
+      </c>
+      <c r="F87" t="s">
+        <v>360</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H87" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>361</v>
+      </c>
+      <c r="B88" t="s">
+        <v>362</v>
+      </c>
+      <c r="C88" t="s">
+        <v>363</v>
+      </c>
+      <c r="D88" t="s">
+        <v>364</v>
+      </c>
+      <c r="E88" t="s">
+        <v>365</v>
+      </c>
+      <c r="F88" t="s">
+        <v>362</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H88" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>366</v>
+      </c>
+      <c r="B89" t="s">
+        <v>367</v>
+      </c>
+      <c r="C89" t="s">
+        <v>368</v>
+      </c>
+      <c r="D89" t="s">
+        <v>369</v>
+      </c>
+      <c r="E89" t="s">
+        <v>370</v>
+      </c>
+      <c r="F89" t="s">
+        <v>371</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H89" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>372</v>
+      </c>
+      <c r="B90">
+        <v>10101100</v>
+      </c>
+      <c r="C90">
+        <v>11000000</v>
+      </c>
+      <c r="D90">
+        <v>1111111</v>
+      </c>
+      <c r="E90">
+        <v>10101000</v>
+      </c>
+      <c r="F90">
+        <v>11000000</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H90" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>373</v>
+      </c>
+      <c r="B91" t="s">
+        <v>374</v>
+      </c>
+      <c r="C91" t="s">
+        <v>375</v>
+      </c>
+      <c r="D91" t="s">
+        <v>376</v>
+      </c>
+      <c r="E91" t="s">
+        <v>377</v>
+      </c>
+      <c r="F91" t="s">
+        <v>374</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H91" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>372</v>
+      </c>
+      <c r="B92">
+        <v>168</v>
+      </c>
+      <c r="C92">
+        <v>172</v>
+      </c>
+      <c r="D92">
+        <v>192</v>
+      </c>
+      <c r="E92">
+        <v>255</v>
+      </c>
+      <c r="F92">
+        <v>172</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H92" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>378</v>
+      </c>
+      <c r="B93" t="s">
+        <v>379</v>
+      </c>
+      <c r="C93" t="s">
+        <v>381</v>
+      </c>
+      <c r="D93" t="s">
+        <v>382</v>
+      </c>
+      <c r="E93" t="s">
+        <v>380</v>
+      </c>
+      <c r="F93" t="s">
+        <v>380</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H93" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>383</v>
+      </c>
+      <c r="B94" t="s">
+        <v>387</v>
+      </c>
+      <c r="C94" t="s">
+        <v>388</v>
+      </c>
+      <c r="D94" t="s">
+        <v>389</v>
+      </c>
+      <c r="E94" t="s">
+        <v>390</v>
+      </c>
+      <c r="F94" t="s">
+        <v>387</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H94" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>383</v>
+      </c>
+      <c r="B95" t="s">
+        <v>384</v>
+      </c>
+      <c r="C95" t="s">
+        <v>391</v>
+      </c>
+      <c r="D95" t="s">
+        <v>385</v>
+      </c>
+      <c r="E95" t="s">
+        <v>386</v>
+      </c>
+      <c r="F95" t="s">
+        <v>385</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H95" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>392</v>
+      </c>
+      <c r="B96" t="s">
+        <v>152</v>
+      </c>
+      <c r="C96" t="b">
+        <v>0</v>
+      </c>
+      <c r="F96" t="b">
+        <v>1</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H96" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>393</v>
+      </c>
+      <c r="B97" t="s">
+        <v>394</v>
+      </c>
+      <c r="C97" t="s">
+        <v>395</v>
+      </c>
+      <c r="E97" t="s">
+        <v>396</v>
+      </c>
+      <c r="F97" t="s">
+        <v>395</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H97" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>397</v>
+      </c>
+      <c r="B98" t="s">
+        <v>339</v>
+      </c>
+      <c r="C98" t="s">
+        <v>46</v>
+      </c>
+      <c r="D98" t="s">
+        <v>45</v>
+      </c>
+      <c r="E98" t="s">
+        <v>44</v>
+      </c>
+      <c r="F98" t="s">
+        <v>45</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H98" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>398</v>
+      </c>
+      <c r="B99" t="s">
+        <v>399</v>
+      </c>
+      <c r="C99" t="s">
+        <v>400</v>
+      </c>
+      <c r="D99" t="s">
+        <v>400</v>
+      </c>
+      <c r="E99" t="s">
+        <v>401</v>
+      </c>
+      <c r="F99" t="s">
+        <v>399</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H99" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>402</v>
+      </c>
+      <c r="B100" t="s">
+        <v>399</v>
+      </c>
+      <c r="C100" t="s">
+        <v>400</v>
+      </c>
+      <c r="D100" t="s">
+        <v>403</v>
+      </c>
+      <c r="E100" t="s">
+        <v>401</v>
+      </c>
+      <c r="F100" t="s">
+        <v>404</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H100" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
comitting so i can see updates
yep
</commit_message>
<xml_diff>
--- a/PTA/platforms/browser/www/testBank.xlsx
+++ b/PTA/platforms/browser/www/testBank.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prototype\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Documents\pta\PTA\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="405">
   <si>
     <t>Which of the following is NOT a type of motherboard expansion slot?</t>
   </si>
@@ -477,13 +477,798 @@
   </si>
   <si>
     <t xml:space="preserve">Light Emitting Diode(LED) or Liquid Crystal Displays (LCD) screens are much better at displacing glare than the other technolgy combinations. </t>
+  </si>
+  <si>
+    <r>
+      <t>the main functionality of the basic input/output system (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BIOS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) is to perform the initial hardware checks after the computer is powered on and start up the OS</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">true </t>
+  </si>
+  <si>
+    <t>in modern PCs, the procedure of replacing BIOS contents is sometimes refered to as:</t>
+  </si>
+  <si>
+    <t>hard boot</t>
+  </si>
+  <si>
+    <t>overclock</t>
+  </si>
+  <si>
+    <t>flashing the BIOS</t>
+  </si>
+  <si>
+    <t>Direct memory access DMA</t>
+  </si>
+  <si>
+    <t>Flashing the BIOS</t>
+  </si>
+  <si>
+    <t>A+S</t>
+  </si>
+  <si>
+    <t>which Microsoft Windows OS utility can be used to view basic information about computers BIOS</t>
+  </si>
+  <si>
+    <t>WINVER&gt;EXE</t>
+  </si>
+  <si>
+    <t>MSINFO32.EXE</t>
+  </si>
+  <si>
+    <t>controle panel</t>
+  </si>
+  <si>
+    <t>SERVICES.MSC</t>
+  </si>
+  <si>
+    <t>power failure during BIOS upgrade can be the cause of irreversible damage to the computer system</t>
+  </si>
+  <si>
+    <t>after normal system shutdown, when the computer is turned off, contents of the memory used to store BIOS setting are:</t>
+  </si>
+  <si>
+    <t>Erased</t>
+  </si>
+  <si>
+    <t>Retained</t>
+  </si>
+  <si>
+    <t>Stored in a page file</t>
+  </si>
+  <si>
+    <t>Saved on a harddrive</t>
+  </si>
+  <si>
+    <t>Rettained</t>
+  </si>
+  <si>
+    <t>which of the acronyms listed below refers to a series of basic hardware diagnostic test performed by the BIOS after the computer is powered on?</t>
+  </si>
+  <si>
+    <t>IDE</t>
+  </si>
+  <si>
+    <t>Qos</t>
+  </si>
+  <si>
+    <t>after completing the initial diagnostics and assigning system resources, the startup Bios program checks for information about secondary storage devices that might contain the OS.  The list of devices and the order in which they should be checked can be found and arranged in th CMOS setu utility, and this option is commonly refered to as:</t>
+  </si>
+  <si>
+    <t>boot record</t>
+  </si>
+  <si>
+    <t>Master Boot Record(MBR)</t>
+  </si>
+  <si>
+    <t>Partition table</t>
+  </si>
+  <si>
+    <t>Bootsequence</t>
+  </si>
+  <si>
+    <t>Boot sequence</t>
+  </si>
+  <si>
+    <t>in order to work, an integrated component such as Network Interface Card(NIC) on a newly assembled computer system may need to be first</t>
+  </si>
+  <si>
+    <t>Enabled in Windows Controle Panel</t>
+  </si>
+  <si>
+    <t>Updated with the latest driver in Device Manager</t>
+  </si>
+  <si>
+    <t>Checked against the Hardware Compatibility List (HCL)</t>
+  </si>
+  <si>
+    <t>Enabled in the advances BIOS settings menu</t>
+  </si>
+  <si>
+    <t>Enabled in the advanced BIOS settings menu</t>
+  </si>
+  <si>
+    <t>After launching Windows Virtual PC application technician recives error message stating that the Hardware-Assisted Virtualization(HAV) feature is not enabled on the computer. Which of the folowing steps might help in fixing this problem?</t>
+  </si>
+  <si>
+    <t>increasing the amount of phisical RAM on the system</t>
+  </si>
+  <si>
+    <t>Re-instlling Windows Virtual PC app</t>
+  </si>
+  <si>
+    <t xml:space="preserve">getting into the CMOS setup utility and enabling the virtualization technology setting </t>
+  </si>
+  <si>
+    <t>Safe Mode troubleshooting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Getting the CMOS setup utility and Enabling the virtualization technology setting </t>
+  </si>
+  <si>
+    <t>the CMOS setup utility can be accessed by pressing:</t>
+  </si>
+  <si>
+    <t>Reset button on the front panel of the computer case</t>
+  </si>
+  <si>
+    <t>the key set by the motherboard manufacturer for accessing CMOS setup utility during boot</t>
+  </si>
+  <si>
+    <t>Del key during boot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1 key while loged into Windows </t>
+  </si>
+  <si>
+    <t>Which of the folowing answers refers to a firmware interface designed as a replacement for BIOS?</t>
+  </si>
+  <si>
+    <t>UEFI</t>
+  </si>
+  <si>
+    <t>CMOS</t>
+  </si>
+  <si>
+    <t>USMT</t>
+  </si>
+  <si>
+    <t>Which of the folowing statements is true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aborted BIOS update can be resumed by the transaction recovery system </t>
+  </si>
+  <si>
+    <t>a common securtiy measure is to store BIOS on a non-rewriteable memory chip</t>
+  </si>
+  <si>
+    <t>the process of BIOS update can be aborted and resumed at a later time</t>
+  </si>
+  <si>
+    <t>Aborted BIOS update could render the computer unusable</t>
+  </si>
+  <si>
+    <t>aborted BIOS update could render the computer unusable</t>
+  </si>
+  <si>
+    <t>which type of password provides the hightst level of permissions in BIOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">root </t>
+  </si>
+  <si>
+    <t>supervisor</t>
+  </si>
+  <si>
+    <t>administrator</t>
+  </si>
+  <si>
+    <t>power user</t>
+  </si>
+  <si>
+    <t>what is LoJack?</t>
+  </si>
+  <si>
+    <t>loopback adapter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secutity feature used for locating stolen desktops, laptops, or tablets </t>
+  </si>
+  <si>
+    <t>Conector standard</t>
+  </si>
+  <si>
+    <t>RJ_11 plug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Security feature used for locating stolen Desktops, laptops, or tablets </t>
+  </si>
+  <si>
+    <t>which of the folowing terms refer to a tech that allows for storing passwords, certificates, or encryption keys in a hardware chip?</t>
+  </si>
+  <si>
+    <t>Access Controle List (ACL)</t>
+  </si>
+  <si>
+    <t>Encrypting File System(EFS)</t>
+  </si>
+  <si>
+    <t>User Account Controle (UAC)</t>
+  </si>
+  <si>
+    <t>Trusted Platform Module (TPM)</t>
+  </si>
+  <si>
+    <t>Trusted Platform Module(TPM)</t>
+  </si>
+  <si>
+    <t>while tryign to enable the entire drive encryption feature in windows technician receives the followling error message: "A compatible Trusted Platform Module(TPM) security Device must be present on this computer, but a TPM was not found." knowing that the system had a TPM chip installed, which of the folowing steps might help in solving this problem?</t>
+  </si>
+  <si>
+    <t>Re-install OS</t>
+  </si>
+  <si>
+    <t>Enableing the TPM security feture in CMOS setup menu</t>
+  </si>
+  <si>
+    <t>Hard drive replacement</t>
+  </si>
+  <si>
+    <t>Enabling the TPM security feature in Windows controle panel</t>
+  </si>
+  <si>
+    <t>Enabling the TPM security in CMOS setup menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A computer supporting LoJack tech has two main componets installed: a Application Agent residing in he os which sends tracking signals to the monitoring center allowing the law enforcement to locate and recover stolen device, andd Persistence Module  which restores the Application Agent and allows it to survive os re-installation or hard drive format: the highest level of security offered by LoJack can be achieved when Persistence Module resides in </t>
+  </si>
+  <si>
+    <t>os</t>
+  </si>
+  <si>
+    <t>Partition gap on hard drive</t>
+  </si>
+  <si>
+    <t>Computers BIOS</t>
+  </si>
+  <si>
+    <t>USB key</t>
+  </si>
+  <si>
+    <t>A UEFI functionality designed to prevent the loading of malware and unauthorized Oss during system start-up is known as:</t>
+  </si>
+  <si>
+    <t>LoJack</t>
+  </si>
+  <si>
+    <t>Bitlocker</t>
+  </si>
+  <si>
+    <t>Secure boot</t>
+  </si>
+  <si>
+    <t>Kerberos</t>
+  </si>
+  <si>
+    <t>Similarly to magnetic drives, Solid State-Drives (SSD) require periodic defragmentation in order to improve system performance.</t>
+  </si>
+  <si>
+    <t>a tiny sopt on the LCD monitor display screen that permanetly remains black when it should be activated and displaying color is commonly refered to as stuck pixel.</t>
+  </si>
+  <si>
+    <t>a permanent computer display screen discoloration caused by displaying the same static image for extended periods of time is known as:</t>
+  </si>
+  <si>
+    <t>Artifact</t>
+  </si>
+  <si>
+    <t>Stuck pixel</t>
+  </si>
+  <si>
+    <t>Burn-in</t>
+  </si>
+  <si>
+    <t>Dead pixel</t>
+  </si>
+  <si>
+    <t>which of the folowing command-line utilities allows to test the reachability of a host across an IP network</t>
+  </si>
+  <si>
+    <t>NETSTAT</t>
+  </si>
+  <si>
+    <t>IPCONFIG</t>
+  </si>
+  <si>
+    <t>TRACERT</t>
+  </si>
+  <si>
+    <t>PING</t>
+  </si>
+  <si>
+    <t>NET CONFIG</t>
+  </si>
+  <si>
+    <t>IFCONFIG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">which of the folowing command-line prompt tools listed below allows to display IP addresses, subnet mask, and default gateway for all adaptors? </t>
+  </si>
+  <si>
+    <t>A Linux comand-line utility used for displaying and modifying network interface configuration settings is called</t>
+  </si>
+  <si>
+    <t>NETWORKSETUP</t>
+  </si>
+  <si>
+    <t>Microsoft Windows OS command-line for displaying intermediary points on the packet route is called</t>
+  </si>
+  <si>
+    <t>ROUTE PRINT</t>
+  </si>
+  <si>
+    <t>TRACEOUTE</t>
+  </si>
+  <si>
+    <t>N+</t>
+  </si>
+  <si>
+    <t>which of the folowing is an example of active eavesdropping</t>
+  </si>
+  <si>
+    <t>Phishing</t>
+  </si>
+  <si>
+    <t>DDoS</t>
+  </si>
+  <si>
+    <t>Xmas attack</t>
+  </si>
+  <si>
+    <t>MITM</t>
+  </si>
+  <si>
+    <t>Switch spoofing and double tagging are two primary methods of attacking networked resources on:</t>
+  </si>
+  <si>
+    <t>WLAN</t>
+  </si>
+  <si>
+    <t>VLAN</t>
+  </si>
+  <si>
+    <t>VPN</t>
+  </si>
+  <si>
+    <t>PAN</t>
+  </si>
+  <si>
+    <t>Harmful programs used to disrupt computer operation, gather sensitive information, or gain access to private computer systems are commonly referred to as:</t>
+  </si>
+  <si>
+    <t>Malware</t>
+  </si>
+  <si>
+    <t>Adware</t>
+  </si>
+  <si>
+    <t>Spyware</t>
+  </si>
+  <si>
+    <t>Computer viruses</t>
+  </si>
+  <si>
+    <t>Zero-day attack exploits:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New accounts </t>
+  </si>
+  <si>
+    <t>Packed software</t>
+  </si>
+  <si>
+    <t>well known vulberability</t>
+  </si>
+  <si>
+    <t>Vulnerability that is present in already released software but unknown to the software developer</t>
+  </si>
+  <si>
+    <t>one of the measures for securing network devices includes the practice of disabling unsused ports.</t>
+  </si>
+  <si>
+    <t>a hacker has captured network traffic with cleartext commands sent from the client to the server console. Which of the following ports is being used by the network admin for the client-server communication?</t>
+  </si>
+  <si>
+    <t>which of the folowing answers refers to preferred replacement for SLIP protocol</t>
+  </si>
+  <si>
+    <t>PPP</t>
+  </si>
+  <si>
+    <t>PoE</t>
+  </si>
+  <si>
+    <t>CHAP</t>
+  </si>
+  <si>
+    <t>PAP</t>
+  </si>
+  <si>
+    <t>FTPS is an extension to the Secure Shell Protocol (SSH) and runs by default on port number 22</t>
+  </si>
+  <si>
+    <t>which of the following protocols does not provide authentication?</t>
+  </si>
+  <si>
+    <t>FTP</t>
+  </si>
+  <si>
+    <t>SCP</t>
+  </si>
+  <si>
+    <t>TFTP</t>
+  </si>
+  <si>
+    <t>SFTP</t>
+  </si>
+  <si>
+    <t>of the three exsiting versions of the Simple Network Management Protocol (SNMP) versions 1 and 2 (SNMPv1 and SNMPv2) offer authentication based on community strings sent in an unencrypted form (in cleartext). SNMPv3 provides packet encryption, authentication, and hasning mechanisms that allow for checking whether data has changed in transit.</t>
+  </si>
+  <si>
+    <t>which of the following answers refers to a cryptographic network protocol for secure data communication, remote command-line login, remote command execution, and other secure network services between computers?</t>
+  </si>
+  <si>
+    <t>Telnet</t>
+  </si>
+  <si>
+    <t>SSH</t>
+  </si>
+  <si>
+    <t>Bcrypt</t>
+  </si>
+  <si>
+    <t>which of the protocols listed below was designed as a secure replacement for Telnet</t>
+  </si>
+  <si>
+    <t>LDAP</t>
+  </si>
+  <si>
+    <t>the SCP protocol is used for:</t>
+  </si>
+  <si>
+    <t>Directory access</t>
+  </si>
+  <si>
+    <t>Secure file transfer</t>
+  </si>
+  <si>
+    <t>Network addressing</t>
+  </si>
+  <si>
+    <t>Sending emails</t>
+  </si>
+  <si>
+    <t>Which ot the Ipsec modes provides entire packet encryption?</t>
+  </si>
+  <si>
+    <t>Tunnel</t>
+  </si>
+  <si>
+    <t>Payload</t>
+  </si>
+  <si>
+    <t>Transport</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>which of the following solutions provides a shielded environment that protects against unintentional signal leakage and eavesdropping</t>
+  </si>
+  <si>
+    <t>SCADA</t>
+  </si>
+  <si>
+    <t>TEMPEST</t>
+  </si>
+  <si>
+    <t>HVAC</t>
+  </si>
+  <si>
+    <t>RADIUS</t>
+  </si>
+  <si>
+    <t>Data files containing detection and remediation code that antivirus or antispyware products use to identify malicious code are known as</t>
+  </si>
+  <si>
+    <t>Repositories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">signature files </t>
+  </si>
+  <si>
+    <t>macros</t>
+  </si>
+  <si>
+    <t>Security logs</t>
+  </si>
+  <si>
+    <t>signature files</t>
+  </si>
+  <si>
+    <t>the term "DHCP snooping" refers to an exploit that enables operation of a rouge DHCP server on a network.</t>
+  </si>
+  <si>
+    <t>Simple Mail Transfer Protocol(SMTP) operates with the use of TCP port:</t>
+  </si>
+  <si>
+    <t>Which of the potr numbers listed below is commonly used for Session Iniation Protocol (SIP) non-encrypted traffic?</t>
+  </si>
+  <si>
+    <t>Port number 5061 is typically used for Session Initiation Protocol (SIP) traffic encrypted with Transport Layre Security (TLS)</t>
+  </si>
+  <si>
+    <t>port number 5004 is used by:</t>
+  </si>
+  <si>
+    <t>MGCP</t>
+  </si>
+  <si>
+    <t>RTP</t>
+  </si>
+  <si>
+    <t>H.323</t>
+  </si>
+  <si>
+    <t>RTCP</t>
+  </si>
+  <si>
+    <t>RTP contorl Protocol RTCP runs by defalt on port</t>
+  </si>
+  <si>
+    <t>TCP port 1720 is the default port number for</t>
+  </si>
+  <si>
+    <t>PPTP</t>
+  </si>
+  <si>
+    <t>User Datagram Protocol (UDP) is a connection- oriented protocol that requires a set of initial steps in order to establish a connection, supports retransmission of lost packets, flow control, or sequencing</t>
+  </si>
+  <si>
+    <t>Transmission Controle Protocol(tcp) is an example of connectionless protocol. TCP doesn’t support three-way handshake</t>
+  </si>
+  <si>
+    <t>Which of the following protocols is used in network management systems for monitoring network- attached devices?</t>
+  </si>
+  <si>
+    <t>IMAP</t>
+  </si>
+  <si>
+    <t>SNMP</t>
+  </si>
+  <si>
+    <t>An SNMP Agent recives request on UDP port:</t>
+  </si>
+  <si>
+    <t>Which of the following answers lists a cryptographic network protocol for secure data communication, remote command-line login, remote command execution, and other secure network services between two networked computers?</t>
+  </si>
+  <si>
+    <t>A hacker has captured network traffic with cleartext commands sent from the client to the server console. Which of the following ports is being used by the network admin for the client-server communication?</t>
+  </si>
+  <si>
+    <t>A network administrator wants to replace a service running on port 23 with a more reliable solution. Which of the following ports would be in use after implementing this change?</t>
+  </si>
+  <si>
+    <t>DNS runs on port:</t>
+  </si>
+  <si>
+    <t>UDP port 67 is used by:</t>
+  </si>
+  <si>
+    <t>Bootstrap Protocol(BOOTP)</t>
+  </si>
+  <si>
+    <t>remote authentication Dial in user service (RADIUS)</t>
+  </si>
+  <si>
+    <t>Simple Network Management Protocol SNMP</t>
+  </si>
+  <si>
+    <t>Merberos</t>
+  </si>
+  <si>
+    <t>which of the file transfer protocols listed below runs on port number 69 and does not provide authentication?</t>
+  </si>
+  <si>
+    <t>TCP port 445 is used by:</t>
+  </si>
+  <si>
+    <t>RDP</t>
+  </si>
+  <si>
+    <t>SMB</t>
+  </si>
+  <si>
+    <t>SIP</t>
+  </si>
+  <si>
+    <t>A network technician uses an RDP client on their Windows OS in order to remotely troubleshoot a problem on another Windows machine. Which of the following ports needs to be opened for the built-in Windows RDP server to allow this type of network connection?</t>
+  </si>
+  <si>
+    <t>A double colon in an IPv6 address indicates that part of the address containing only zeroes has been compressed to make the address shorter</t>
+  </si>
+  <si>
+    <t>Which of the following answers lists a valid address of FE80:0000:0000:0000:02AA:0000:4C00:FE9A after compression?</t>
+  </si>
+  <si>
+    <t>FE80::2AA::4C00:FE9A</t>
+  </si>
+  <si>
+    <t>FE80:0:2AA:0:4C:FE9A</t>
+  </si>
+  <si>
+    <t>FE80:0:02AA::4C:FE9A</t>
+  </si>
+  <si>
+    <t>An IPv4 to IPv6 transition mechanism that allows IPv6 packets to be transmitted over an IPv4 network is known as:</t>
+  </si>
+  <si>
+    <t>6to4</t>
+  </si>
+  <si>
+    <t>802.3af</t>
+  </si>
+  <si>
+    <t>eDiscovery</t>
+  </si>
+  <si>
+    <t>Miredo</t>
+  </si>
+  <si>
+    <t>What does the term "Miredo" refer to?</t>
+  </si>
+  <si>
+    <t>IPv4 to IPV6 migration mechanism</t>
+  </si>
+  <si>
+    <t>Load balancing solution</t>
+  </si>
+  <si>
+    <t>TeredoIPv6</t>
+  </si>
+  <si>
+    <t>Content filtering solution</t>
+  </si>
+  <si>
+    <t>Teredo IPv6 tunneling software</t>
+  </si>
+  <si>
+    <t>Which of the following answers lists the binary notation of the decimal number 192?</t>
+  </si>
+  <si>
+    <t>an Ipv 4 address consists of:</t>
+  </si>
+  <si>
+    <t>32bits</t>
+  </si>
+  <si>
+    <t>48bits</t>
+  </si>
+  <si>
+    <t>64bits</t>
+  </si>
+  <si>
+    <t>128bits</t>
+  </si>
+  <si>
+    <t>Which of the following is an example of a valid subnet mask?</t>
+  </si>
+  <si>
+    <t>255.255.225.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None of the above is a valid subnet mask </t>
+  </si>
+  <si>
+    <t>255.255.191.0</t>
+  </si>
+  <si>
+    <t>255.255.64.0</t>
+  </si>
+  <si>
+    <t>Which of the following answers lists the default (classful) subnet mask for a class A network?</t>
+  </si>
+  <si>
+    <t>192.168.0.3</t>
+  </si>
+  <si>
+    <t>169.254.10.20</t>
+  </si>
+  <si>
+    <t>65.55.57.27</t>
+  </si>
+  <si>
+    <t>255.0.0.0</t>
+  </si>
+  <si>
+    <t>255.128.0.0</t>
+  </si>
+  <si>
+    <t>224.0.0.0</t>
+  </si>
+  <si>
+    <t>255.244.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 127.0.0.1 </t>
+  </si>
+  <si>
+    <t>APIPA-assigned addresses are valid only for communications within a network segment that a given host is connected to (a host with APIPA-assigned address cannot connect to the Internet).</t>
+  </si>
+  <si>
+    <t>Which of the following answers lists the default (classful) subnet mask for a class C network?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">255.255.192.0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">255.255.224.0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">255.255.252.0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> An IPv4 address in the range 169.254.1.0 through 169.254.254.255 indicates a problem with what type of service?</t>
+  </si>
+  <si>
+    <t>In IPv4 addressing, the leading octet of an IP address with a value of 1 through 126 denotes that the IP address within that range belongs to the:</t>
+  </si>
+  <si>
+    <t>Class A address space</t>
+  </si>
+  <si>
+    <t>Class B address space</t>
+  </si>
+  <si>
+    <t>Class D address space</t>
+  </si>
+  <si>
+    <t>In IPv4 addressing, the leading octet of an IP address with a value of 192 through 223 denotes that the IP address within that range belongs to the:</t>
+  </si>
+  <si>
+    <t>Class C Address space</t>
+  </si>
+  <si>
+    <t>Class C address space</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -492,6 +1277,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF333333"/>
       <name val="Calibri"/>
@@ -837,10 +1630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="B74" workbookViewId="0">
+      <selection activeCell="G100" sqref="G100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1501,68 +2294,1647 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C26" t="b">
+        <v>0</v>
+      </c>
+      <c r="F26" t="b">
+        <v>1</v>
+      </c>
       <c r="H26" t="s">
-        <v>6</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="H27" t="s">
-        <v>6</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>162</v>
+      </c>
       <c r="H28" t="s">
-        <v>6</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C29" t="b">
+        <v>0</v>
+      </c>
+      <c r="F29" t="b">
+        <v>1</v>
+      </c>
       <c r="H29" t="s">
-        <v>6</v>
+        <v>159</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>171</v>
+      </c>
       <c r="H30" t="s">
-        <v>6</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="H31" t="s">
-        <v>6</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>180</v>
+      </c>
       <c r="H32" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="8:8" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>186</v>
+      </c>
       <c r="H33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="8:8" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>192</v>
+      </c>
       <c r="H34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="8:8" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>195</v>
+      </c>
       <c r="H35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="8:8" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>199</v>
+      </c>
       <c r="H36" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="8:8" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>207</v>
+      </c>
       <c r="H37" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="8:8" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>210</v>
+      </c>
       <c r="H38" t="s">
-        <v>6</v>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C44" t="b">
+        <v>0</v>
+      </c>
+      <c r="F44" t="b">
+        <v>0</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C45" t="b">
+        <v>0</v>
+      </c>
+      <c r="F45" t="b">
+        <v>0</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="H53" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F54" t="s">
+        <v>281</v>
+      </c>
+      <c r="H54" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F55" t="b">
+        <v>1</v>
+      </c>
+      <c r="H55" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B56">
+        <v>49</v>
+      </c>
+      <c r="C56">
+        <v>23</v>
+      </c>
+      <c r="D56">
+        <v>68</v>
+      </c>
+      <c r="E56">
+        <v>22</v>
+      </c>
+      <c r="F56">
+        <v>23</v>
+      </c>
+      <c r="H56" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="H57" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C58" t="b">
+        <v>0</v>
+      </c>
+      <c r="F58" t="b">
+        <v>1</v>
+      </c>
+      <c r="H58" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C59" t="s">
+        <v>292</v>
+      </c>
+      <c r="D59" t="s">
+        <v>293</v>
+      </c>
+      <c r="E59" t="s">
+        <v>294</v>
+      </c>
+      <c r="F59" t="s">
+        <v>293</v>
+      </c>
+      <c r="H59" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C60" t="b">
+        <v>0</v>
+      </c>
+      <c r="F60" t="b">
+        <v>1</v>
+      </c>
+      <c r="H60" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C61" t="s">
+        <v>298</v>
+      </c>
+      <c r="D61" t="s">
+        <v>299</v>
+      </c>
+      <c r="E61" t="s">
+        <v>293</v>
+      </c>
+      <c r="F61" t="s">
+        <v>298</v>
+      </c>
+      <c r="H61" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C62" t="s">
+        <v>301</v>
+      </c>
+      <c r="D62" t="s">
+        <v>291</v>
+      </c>
+      <c r="E62" t="s">
+        <v>287</v>
+      </c>
+      <c r="F62" t="s">
+        <v>298</v>
+      </c>
+      <c r="H62" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C63" t="s">
+        <v>304</v>
+      </c>
+      <c r="D63" t="s">
+        <v>305</v>
+      </c>
+      <c r="E63" t="s">
+        <v>306</v>
+      </c>
+      <c r="F63" t="s">
+        <v>304</v>
+      </c>
+      <c r="H63" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C64" t="s">
+        <v>309</v>
+      </c>
+      <c r="D64" t="s">
+        <v>310</v>
+      </c>
+      <c r="E64" t="s">
+        <v>311</v>
+      </c>
+      <c r="F64" t="s">
+        <v>308</v>
+      </c>
+      <c r="H64" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C65" t="s">
+        <v>313</v>
+      </c>
+      <c r="D65" t="s">
+        <v>315</v>
+      </c>
+      <c r="E65" t="s">
+        <v>316</v>
+      </c>
+      <c r="F65" t="s">
+        <v>314</v>
+      </c>
+      <c r="H65" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C66" t="s">
+        <v>319</v>
+      </c>
+      <c r="D66" t="s">
+        <v>320</v>
+      </c>
+      <c r="E66" t="s">
+        <v>321</v>
+      </c>
+      <c r="F66" t="s">
+        <v>322</v>
+      </c>
+      <c r="H66" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C67" t="b">
+        <v>0</v>
+      </c>
+      <c r="F67" t="b">
+        <v>0</v>
+      </c>
+      <c r="H67" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B68">
+        <v>110</v>
+      </c>
+      <c r="C68">
+        <v>23</v>
+      </c>
+      <c r="D68">
+        <v>143</v>
+      </c>
+      <c r="E68">
+        <v>25</v>
+      </c>
+      <c r="F68">
+        <v>25</v>
+      </c>
+      <c r="H68" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B69">
+        <v>5004</v>
+      </c>
+      <c r="C69">
+        <v>5005</v>
+      </c>
+      <c r="D69">
+        <v>5060</v>
+      </c>
+      <c r="E69">
+        <v>5061</v>
+      </c>
+      <c r="F69">
+        <v>5060</v>
+      </c>
+      <c r="H69" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C70" t="b">
+        <v>0</v>
+      </c>
+      <c r="F70" t="b">
+        <v>0</v>
+      </c>
+      <c r="H70" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C71" t="s">
+        <v>329</v>
+      </c>
+      <c r="D71" t="s">
+        <v>330</v>
+      </c>
+      <c r="E71" t="s">
+        <v>331</v>
+      </c>
+      <c r="F71" t="s">
+        <v>329</v>
+      </c>
+      <c r="H71" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B72">
+        <v>5004</v>
+      </c>
+      <c r="C72">
+        <v>5060</v>
+      </c>
+      <c r="D72">
+        <v>5005</v>
+      </c>
+      <c r="E72">
+        <v>5061</v>
+      </c>
+      <c r="F72">
+        <v>5005</v>
+      </c>
+      <c r="H72" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B73" t="s">
+        <v>328</v>
+      </c>
+      <c r="C73" t="s">
+        <v>330</v>
+      </c>
+      <c r="D73" t="s">
+        <v>334</v>
+      </c>
+      <c r="E73" t="s">
+        <v>329</v>
+      </c>
+      <c r="F73" t="s">
+        <v>330</v>
+      </c>
+      <c r="H73" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B74" t="s">
+        <v>152</v>
+      </c>
+      <c r="C74" t="b">
+        <v>0</v>
+      </c>
+      <c r="F74" t="b">
+        <v>0</v>
+      </c>
+      <c r="H74" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B75" t="s">
+        <v>152</v>
+      </c>
+      <c r="C75" t="b">
+        <v>0</v>
+      </c>
+      <c r="F75" t="b">
+        <v>0</v>
+      </c>
+      <c r="H75" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B76" t="s">
+        <v>329</v>
+      </c>
+      <c r="C76" t="s">
+        <v>338</v>
+      </c>
+      <c r="D76" t="s">
+        <v>339</v>
+      </c>
+      <c r="E76" t="s">
+        <v>331</v>
+      </c>
+      <c r="F76" t="s">
+        <v>339</v>
+      </c>
+      <c r="H76" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B77">
+        <v>161</v>
+      </c>
+      <c r="C77">
+        <v>138</v>
+      </c>
+      <c r="D77">
+        <v>162</v>
+      </c>
+      <c r="E77">
+        <v>139</v>
+      </c>
+      <c r="F77">
+        <v>161</v>
+      </c>
+      <c r="H77" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B78" t="s">
+        <v>297</v>
+      </c>
+      <c r="C78" t="s">
+        <v>298</v>
+      </c>
+      <c r="D78" t="s">
+        <v>299</v>
+      </c>
+      <c r="E78" t="s">
+        <v>293</v>
+      </c>
+      <c r="F78" t="s">
+        <v>298</v>
+      </c>
+      <c r="H78" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>342</v>
+      </c>
+      <c r="B79">
+        <v>49</v>
+      </c>
+      <c r="C79">
+        <v>23</v>
+      </c>
+      <c r="D79">
+        <v>68</v>
+      </c>
+      <c r="E79">
+        <v>22</v>
+      </c>
+      <c r="F79">
+        <v>23</v>
+      </c>
+      <c r="H79" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>343</v>
+      </c>
+      <c r="B80">
+        <v>20</v>
+      </c>
+      <c r="C80">
+        <v>21</v>
+      </c>
+      <c r="D80">
+        <v>22</v>
+      </c>
+      <c r="E80">
+        <v>25</v>
+      </c>
+      <c r="F80">
+        <v>22</v>
+      </c>
+      <c r="H80" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B81">
+        <v>139</v>
+      </c>
+      <c r="C81">
+        <v>53</v>
+      </c>
+      <c r="D81">
+        <v>443</v>
+      </c>
+      <c r="E81">
+        <v>22</v>
+      </c>
+      <c r="F81">
+        <v>53</v>
+      </c>
+      <c r="H81" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B82" t="s">
+        <v>346</v>
+      </c>
+      <c r="C82" t="s">
+        <v>347</v>
+      </c>
+      <c r="D82" t="s">
+        <v>348</v>
+      </c>
+      <c r="E82" t="s">
+        <v>349</v>
+      </c>
+      <c r="F82" t="s">
+        <v>346</v>
+      </c>
+      <c r="H82" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B83" t="s">
+        <v>291</v>
+      </c>
+      <c r="C83" t="s">
+        <v>293</v>
+      </c>
+      <c r="D83" t="s">
+        <v>292</v>
+      </c>
+      <c r="E83" t="s">
+        <v>294</v>
+      </c>
+      <c r="F83" t="s">
+        <v>293</v>
+      </c>
+      <c r="H83" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B84" t="s">
+        <v>352</v>
+      </c>
+      <c r="C84" t="s">
+        <v>353</v>
+      </c>
+      <c r="D84" t="s">
+        <v>354</v>
+      </c>
+      <c r="E84" t="s">
+        <v>329</v>
+      </c>
+      <c r="F84" t="s">
+        <v>353</v>
+      </c>
+      <c r="H84" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>355</v>
+      </c>
+      <c r="B85">
+        <v>1701</v>
+      </c>
+      <c r="C85">
+        <v>139</v>
+      </c>
+      <c r="D85">
+        <v>3389</v>
+      </c>
+      <c r="E85">
+        <v>110</v>
+      </c>
+      <c r="F85">
+        <v>3389</v>
+      </c>
+      <c r="H85" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>356</v>
+      </c>
+      <c r="B86" t="s">
+        <v>152</v>
+      </c>
+      <c r="C86" t="b">
+        <v>0</v>
+      </c>
+      <c r="F86" t="b">
+        <v>1</v>
+      </c>
+      <c r="H86" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>357</v>
+      </c>
+      <c r="B87" t="s">
+        <v>358</v>
+      </c>
+      <c r="C87" t="s">
+        <v>359</v>
+      </c>
+      <c r="D87" t="s">
+        <v>359</v>
+      </c>
+      <c r="E87" t="s">
+        <v>360</v>
+      </c>
+      <c r="F87" t="s">
+        <v>360</v>
+      </c>
+      <c r="H87" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>361</v>
+      </c>
+      <c r="B88" t="s">
+        <v>362</v>
+      </c>
+      <c r="C88" t="s">
+        <v>363</v>
+      </c>
+      <c r="D88" t="s">
+        <v>364</v>
+      </c>
+      <c r="E88" t="s">
+        <v>365</v>
+      </c>
+      <c r="F88" t="s">
+        <v>362</v>
+      </c>
+      <c r="H88" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>366</v>
+      </c>
+      <c r="B89" t="s">
+        <v>367</v>
+      </c>
+      <c r="C89" t="s">
+        <v>368</v>
+      </c>
+      <c r="D89" t="s">
+        <v>369</v>
+      </c>
+      <c r="E89" t="s">
+        <v>370</v>
+      </c>
+      <c r="F89" t="s">
+        <v>371</v>
+      </c>
+      <c r="H89" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>372</v>
+      </c>
+      <c r="B90">
+        <v>10101100</v>
+      </c>
+      <c r="C90">
+        <v>11000000</v>
+      </c>
+      <c r="D90">
+        <v>1111111</v>
+      </c>
+      <c r="E90">
+        <v>10101000</v>
+      </c>
+      <c r="F90">
+        <v>11000000</v>
+      </c>
+      <c r="H90" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>373</v>
+      </c>
+      <c r="B91" t="s">
+        <v>374</v>
+      </c>
+      <c r="C91" t="s">
+        <v>375</v>
+      </c>
+      <c r="D91" t="s">
+        <v>376</v>
+      </c>
+      <c r="E91" t="s">
+        <v>377</v>
+      </c>
+      <c r="F91" t="s">
+        <v>374</v>
+      </c>
+      <c r="H91" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>372</v>
+      </c>
+      <c r="B92">
+        <v>168</v>
+      </c>
+      <c r="C92">
+        <v>172</v>
+      </c>
+      <c r="D92">
+        <v>192</v>
+      </c>
+      <c r="E92">
+        <v>255</v>
+      </c>
+      <c r="F92">
+        <v>172</v>
+      </c>
+      <c r="H92" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>378</v>
+      </c>
+      <c r="B93" t="s">
+        <v>379</v>
+      </c>
+      <c r="C93" t="s">
+        <v>381</v>
+      </c>
+      <c r="D93" t="s">
+        <v>382</v>
+      </c>
+      <c r="E93" t="s">
+        <v>380</v>
+      </c>
+      <c r="F93" t="s">
+        <v>380</v>
+      </c>
+      <c r="H93" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>383</v>
+      </c>
+      <c r="B94" t="s">
+        <v>387</v>
+      </c>
+      <c r="C94" t="s">
+        <v>388</v>
+      </c>
+      <c r="D94" t="s">
+        <v>389</v>
+      </c>
+      <c r="E94" t="s">
+        <v>390</v>
+      </c>
+      <c r="F94" t="s">
+        <v>387</v>
+      </c>
+      <c r="H94" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>383</v>
+      </c>
+      <c r="B95" t="s">
+        <v>384</v>
+      </c>
+      <c r="C95" t="s">
+        <v>391</v>
+      </c>
+      <c r="D95" t="s">
+        <v>385</v>
+      </c>
+      <c r="E95" t="s">
+        <v>386</v>
+      </c>
+      <c r="F95" t="s">
+        <v>385</v>
+      </c>
+      <c r="H95" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>392</v>
+      </c>
+      <c r="B96" t="s">
+        <v>152</v>
+      </c>
+      <c r="C96" t="b">
+        <v>0</v>
+      </c>
+      <c r="F96" t="b">
+        <v>1</v>
+      </c>
+      <c r="H96" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>393</v>
+      </c>
+      <c r="B97" t="s">
+        <v>394</v>
+      </c>
+      <c r="C97" t="s">
+        <v>395</v>
+      </c>
+      <c r="E97" t="s">
+        <v>396</v>
+      </c>
+      <c r="F97" t="s">
+        <v>395</v>
+      </c>
+      <c r="H97" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>397</v>
+      </c>
+      <c r="B98" t="s">
+        <v>339</v>
+      </c>
+      <c r="C98" t="s">
+        <v>46</v>
+      </c>
+      <c r="D98" t="s">
+        <v>45</v>
+      </c>
+      <c r="E98" t="s">
+        <v>44</v>
+      </c>
+      <c r="F98" t="s">
+        <v>45</v>
+      </c>
+      <c r="H98" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>398</v>
+      </c>
+      <c r="B99" t="s">
+        <v>399</v>
+      </c>
+      <c r="C99" t="s">
+        <v>400</v>
+      </c>
+      <c r="D99" t="s">
+        <v>400</v>
+      </c>
+      <c r="E99" t="s">
+        <v>401</v>
+      </c>
+      <c r="F99" t="s">
+        <v>399</v>
+      </c>
+      <c r="H99" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>402</v>
+      </c>
+      <c r="B100" t="s">
+        <v>399</v>
+      </c>
+      <c r="C100" t="s">
+        <v>400</v>
+      </c>
+      <c r="D100" t="s">
+        <v>403</v>
+      </c>
+      <c r="E100" t="s">
+        <v>401</v>
+      </c>
+      <c r="F100" t="s">
+        <v>404</v>
+      </c>
+      <c r="H100" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remembers selection on submit
</commit_message>
<xml_diff>
--- a/PTA/platforms/browser/www/testBank.xlsx
+++ b/PTA/platforms/browser/www/testBank.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Documents\pta\PTA\www\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calvin\Documents\PTAlso\PTA\PTA\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="406">
   <si>
     <t>Which of the following is NOT a type of motherboard expansion slot?</t>
   </si>
@@ -1262,6 +1262,9 @@
   </si>
   <si>
     <t>Class C address space</t>
+  </si>
+  <si>
+    <t>I'm sure you know why (Placeholder)</t>
   </si>
 </sst>
 </file>
@@ -1632,8 +1635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B74" workbookViewId="0">
-      <selection activeCell="G100" sqref="G100"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="G105" sqref="G105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2306,6 +2309,9 @@
       <c r="F26" t="b">
         <v>1</v>
       </c>
+      <c r="G26" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H26" t="s">
         <v>159</v>
       </c>
@@ -2329,6 +2335,9 @@
       <c r="F27" s="1" t="s">
         <v>158</v>
       </c>
+      <c r="G27" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H27" t="s">
         <v>159</v>
       </c>
@@ -2352,6 +2361,9 @@
       <c r="F28" s="1" t="s">
         <v>162</v>
       </c>
+      <c r="G28" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H28" t="s">
         <v>159</v>
       </c>
@@ -2369,6 +2381,9 @@
       <c r="F29" t="b">
         <v>1</v>
       </c>
+      <c r="G29" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H29" t="s">
         <v>159</v>
       </c>
@@ -2392,6 +2407,9 @@
       <c r="F30" s="1" t="s">
         <v>171</v>
       </c>
+      <c r="G30" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H30" t="s">
         <v>159</v>
       </c>
@@ -2415,6 +2433,9 @@
       <c r="F31" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="G31" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H31" t="s">
         <v>159</v>
       </c>
@@ -2438,6 +2459,9 @@
       <c r="F32" s="1" t="s">
         <v>180</v>
       </c>
+      <c r="G32" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H32" t="s">
         <v>159</v>
       </c>
@@ -2461,6 +2485,9 @@
       <c r="F33" s="1" t="s">
         <v>186</v>
       </c>
+      <c r="G33" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H33" t="s">
         <v>159</v>
       </c>
@@ -2484,6 +2511,9 @@
       <c r="F34" s="1" t="s">
         <v>192</v>
       </c>
+      <c r="G34" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H34" t="s">
         <v>159</v>
       </c>
@@ -2507,6 +2537,9 @@
       <c r="F35" s="1" t="s">
         <v>195</v>
       </c>
+      <c r="G35" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H35" t="s">
         <v>159</v>
       </c>
@@ -2530,6 +2563,9 @@
       <c r="F36" s="1" t="s">
         <v>199</v>
       </c>
+      <c r="G36" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H36" t="s">
         <v>159</v>
       </c>
@@ -2553,6 +2589,9 @@
       <c r="F37" s="1" t="s">
         <v>207</v>
       </c>
+      <c r="G37" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H37" t="s">
         <v>159</v>
       </c>
@@ -2576,6 +2615,9 @@
       <c r="F38" s="1" t="s">
         <v>210</v>
       </c>
+      <c r="G38" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H38" t="s">
         <v>159</v>
       </c>
@@ -2599,6 +2641,9 @@
       <c r="F39" s="1" t="s">
         <v>218</v>
       </c>
+      <c r="G39" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H39" s="1" t="s">
         <v>159</v>
       </c>
@@ -2622,6 +2667,9 @@
       <c r="F40" s="1" t="s">
         <v>224</v>
       </c>
+      <c r="G40" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H40" s="1" t="s">
         <v>159</v>
       </c>
@@ -2645,6 +2693,9 @@
       <c r="F41" s="1" t="s">
         <v>230</v>
       </c>
+      <c r="G41" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H41" s="1" t="s">
         <v>159</v>
       </c>
@@ -2668,6 +2719,9 @@
       <c r="F42" s="1" t="s">
         <v>234</v>
       </c>
+      <c r="G42" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H42" s="1" t="s">
         <v>159</v>
       </c>
@@ -2691,6 +2745,9 @@
       <c r="F43" s="1" t="s">
         <v>239</v>
       </c>
+      <c r="G43" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H43" s="1" t="s">
         <v>159</v>
       </c>
@@ -2708,6 +2765,9 @@
       <c r="F44" t="b">
         <v>0</v>
       </c>
+      <c r="G44" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H44" s="1" t="s">
         <v>159</v>
       </c>
@@ -2725,6 +2785,9 @@
       <c r="F45" t="b">
         <v>0</v>
       </c>
+      <c r="G45" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H45" s="1" t="s">
         <v>159</v>
       </c>
@@ -2748,6 +2811,9 @@
       <c r="F46" s="1" t="s">
         <v>246</v>
       </c>
+      <c r="G46" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H46" s="1" t="s">
         <v>159</v>
       </c>
@@ -2771,6 +2837,9 @@
       <c r="F47" s="1" t="s">
         <v>252</v>
       </c>
+      <c r="G47" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H47" s="1" t="s">
         <v>159</v>
       </c>
@@ -2794,6 +2863,9 @@
       <c r="F48" s="1" t="s">
         <v>250</v>
       </c>
+      <c r="G48" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H48" s="1" t="s">
         <v>159</v>
       </c>
@@ -2817,6 +2889,9 @@
       <c r="F49" s="1" t="s">
         <v>254</v>
       </c>
+      <c r="G49" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H49" s="1" t="s">
         <v>159</v>
       </c>
@@ -2840,6 +2915,9 @@
       <c r="F50" s="1" t="s">
         <v>251</v>
       </c>
+      <c r="G50" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H50" s="1" t="s">
         <v>159</v>
       </c>
@@ -2863,6 +2941,9 @@
       <c r="F51" s="1" t="s">
         <v>266</v>
       </c>
+      <c r="G51" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H51" s="1" t="s">
         <v>261</v>
       </c>
@@ -2886,6 +2967,9 @@
       <c r="F52" s="1" t="s">
         <v>269</v>
       </c>
+      <c r="G52" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H52" s="1" t="s">
         <v>261</v>
       </c>
@@ -2909,6 +2993,9 @@
       <c r="F53" s="1" t="s">
         <v>273</v>
       </c>
+      <c r="G53" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H53" t="s">
         <v>261</v>
       </c>
@@ -2932,6 +3019,9 @@
       <c r="F54" t="s">
         <v>281</v>
       </c>
+      <c r="G54" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H54" t="s">
         <v>261</v>
       </c>
@@ -2949,6 +3039,9 @@
       <c r="F55" t="b">
         <v>1</v>
       </c>
+      <c r="G55" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H55" t="s">
         <v>261</v>
       </c>
@@ -2972,6 +3065,9 @@
       <c r="F56">
         <v>23</v>
       </c>
+      <c r="G56" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H56" t="s">
         <v>261</v>
       </c>
@@ -2995,6 +3091,9 @@
       <c r="F57" s="1" t="s">
         <v>285</v>
       </c>
+      <c r="G57" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H57" t="s">
         <v>261</v>
       </c>
@@ -3012,6 +3111,9 @@
       <c r="F58" t="b">
         <v>1</v>
       </c>
+      <c r="G58" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H58" t="s">
         <v>261</v>
       </c>
@@ -3035,6 +3137,9 @@
       <c r="F59" t="s">
         <v>293</v>
       </c>
+      <c r="G59" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H59" t="s">
         <v>261</v>
       </c>
@@ -3052,6 +3157,9 @@
       <c r="F60" t="b">
         <v>1</v>
       </c>
+      <c r="G60" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H60" t="s">
         <v>261</v>
       </c>
@@ -3075,6 +3183,9 @@
       <c r="F61" t="s">
         <v>298</v>
       </c>
+      <c r="G61" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H61" t="s">
         <v>261</v>
       </c>
@@ -3098,6 +3209,9 @@
       <c r="F62" t="s">
         <v>298</v>
       </c>
+      <c r="G62" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H62" t="s">
         <v>261</v>
       </c>
@@ -3121,6 +3235,9 @@
       <c r="F63" t="s">
         <v>304</v>
       </c>
+      <c r="G63" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H63" t="s">
         <v>261</v>
       </c>
@@ -3144,6 +3261,9 @@
       <c r="F64" t="s">
         <v>308</v>
       </c>
+      <c r="G64" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H64" t="s">
         <v>261</v>
       </c>
@@ -3167,6 +3287,9 @@
       <c r="F65" t="s">
         <v>314</v>
       </c>
+      <c r="G65" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H65" t="s">
         <v>261</v>
       </c>
@@ -3190,6 +3313,9 @@
       <c r="F66" t="s">
         <v>322</v>
       </c>
+      <c r="G66" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H66" t="s">
         <v>261</v>
       </c>
@@ -3207,6 +3333,9 @@
       <c r="F67" t="b">
         <v>0</v>
       </c>
+      <c r="G67" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H67" t="s">
         <v>261</v>
       </c>
@@ -3230,6 +3359,9 @@
       <c r="F68">
         <v>25</v>
       </c>
+      <c r="G68" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H68" t="s">
         <v>261</v>
       </c>
@@ -3253,6 +3385,9 @@
       <c r="F69">
         <v>5060</v>
       </c>
+      <c r="G69" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H69" t="s">
         <v>261</v>
       </c>
@@ -3270,6 +3405,9 @@
       <c r="F70" t="b">
         <v>0</v>
       </c>
+      <c r="G70" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H70" t="s">
         <v>261</v>
       </c>
@@ -3293,6 +3431,9 @@
       <c r="F71" t="s">
         <v>329</v>
       </c>
+      <c r="G71" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H71" t="s">
         <v>261</v>
       </c>
@@ -3316,6 +3457,9 @@
       <c r="F72">
         <v>5005</v>
       </c>
+      <c r="G72" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H72" t="s">
         <v>261</v>
       </c>
@@ -3339,6 +3483,9 @@
       <c r="F73" t="s">
         <v>330</v>
       </c>
+      <c r="G73" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H73" t="s">
         <v>261</v>
       </c>
@@ -3356,6 +3503,9 @@
       <c r="F74" t="b">
         <v>0</v>
       </c>
+      <c r="G74" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H74" t="s">
         <v>261</v>
       </c>
@@ -3373,6 +3523,9 @@
       <c r="F75" t="b">
         <v>0</v>
       </c>
+      <c r="G75" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H75" t="s">
         <v>261</v>
       </c>
@@ -3396,6 +3549,9 @@
       <c r="F76" t="s">
         <v>339</v>
       </c>
+      <c r="G76" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H76" t="s">
         <v>261</v>
       </c>
@@ -3419,6 +3575,9 @@
       <c r="F77">
         <v>161</v>
       </c>
+      <c r="G77" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H77" t="s">
         <v>261</v>
       </c>
@@ -3442,6 +3601,9 @@
       <c r="F78" t="s">
         <v>298</v>
       </c>
+      <c r="G78" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H78" t="s">
         <v>261</v>
       </c>
@@ -3465,6 +3627,9 @@
       <c r="F79">
         <v>23</v>
       </c>
+      <c r="G79" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H79" t="s">
         <v>261</v>
       </c>
@@ -3488,6 +3653,9 @@
       <c r="F80">
         <v>22</v>
       </c>
+      <c r="G80" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H80" t="s">
         <v>261</v>
       </c>
@@ -3511,6 +3679,9 @@
       <c r="F81">
         <v>53</v>
       </c>
+      <c r="G81" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H81" t="s">
         <v>261</v>
       </c>
@@ -3534,6 +3705,9 @@
       <c r="F82" t="s">
         <v>346</v>
       </c>
+      <c r="G82" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H82" t="s">
         <v>261</v>
       </c>
@@ -3557,6 +3731,9 @@
       <c r="F83" t="s">
         <v>293</v>
       </c>
+      <c r="G83" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H83" t="s">
         <v>261</v>
       </c>
@@ -3580,6 +3757,9 @@
       <c r="F84" t="s">
         <v>353</v>
       </c>
+      <c r="G84" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H84" t="s">
         <v>261</v>
       </c>
@@ -3603,6 +3783,9 @@
       <c r="F85">
         <v>3389</v>
       </c>
+      <c r="G85" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H85" t="s">
         <v>261</v>
       </c>
@@ -3620,6 +3803,9 @@
       <c r="F86" t="b">
         <v>1</v>
       </c>
+      <c r="G86" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H86" t="s">
         <v>261</v>
       </c>
@@ -3643,6 +3829,9 @@
       <c r="F87" t="s">
         <v>360</v>
       </c>
+      <c r="G87" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H87" t="s">
         <v>261</v>
       </c>
@@ -3666,6 +3855,9 @@
       <c r="F88" t="s">
         <v>362</v>
       </c>
+      <c r="G88" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H88" t="s">
         <v>261</v>
       </c>
@@ -3689,6 +3881,9 @@
       <c r="F89" t="s">
         <v>371</v>
       </c>
+      <c r="G89" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H89" t="s">
         <v>261</v>
       </c>
@@ -3712,6 +3907,9 @@
       <c r="F90">
         <v>11000000</v>
       </c>
+      <c r="G90" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H90" t="s">
         <v>261</v>
       </c>
@@ -3735,6 +3933,9 @@
       <c r="F91" t="s">
         <v>374</v>
       </c>
+      <c r="G91" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H91" t="s">
         <v>261</v>
       </c>
@@ -3758,6 +3959,9 @@
       <c r="F92">
         <v>172</v>
       </c>
+      <c r="G92" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H92" t="s">
         <v>261</v>
       </c>
@@ -3781,6 +3985,9 @@
       <c r="F93" t="s">
         <v>380</v>
       </c>
+      <c r="G93" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H93" t="s">
         <v>261</v>
       </c>
@@ -3804,6 +4011,9 @@
       <c r="F94" t="s">
         <v>387</v>
       </c>
+      <c r="G94" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H94" t="s">
         <v>261</v>
       </c>
@@ -3827,6 +4037,9 @@
       <c r="F95" t="s">
         <v>385</v>
       </c>
+      <c r="G95" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H95" t="s">
         <v>261</v>
       </c>
@@ -3844,6 +4057,9 @@
       <c r="F96" t="b">
         <v>1</v>
       </c>
+      <c r="G96" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H96" t="s">
         <v>261</v>
       </c>
@@ -3864,6 +4080,9 @@
       <c r="F97" t="s">
         <v>395</v>
       </c>
+      <c r="G97" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H97" t="s">
         <v>261</v>
       </c>
@@ -3887,6 +4106,9 @@
       <c r="F98" t="s">
         <v>45</v>
       </c>
+      <c r="G98" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H98" t="s">
         <v>261</v>
       </c>
@@ -3910,6 +4132,9 @@
       <c r="F99" t="s">
         <v>399</v>
       </c>
+      <c r="G99" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="H99" t="s">
         <v>261</v>
       </c>
@@ -3932,6 +4157,9 @@
       </c>
       <c r="F100" t="s">
         <v>404</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>405</v>
       </c>
       <c r="H100" t="s">
         <v>261</v>

</xml_diff>

<commit_message>
:+1: updates on modeJS page
</commit_message>
<xml_diff>
--- a/PTA/platforms/browser/www/testBank.xlsx
+++ b/PTA/platforms/browser/www/testBank.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calvin\Documents\PTAlso\PTA\PTA\www\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Documents\pta\PTA\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="653">
   <si>
     <t>Which of the following is NOT a type of motherboard expansion slot?</t>
   </si>
@@ -479,9 +479,6 @@
     <t xml:space="preserve">Light Emitting Diode(LED) or Liquid Crystal Displays (LCD) screens are much better at displacing glare than the other technolgy combinations. </t>
   </si>
   <si>
-    <t>in modern PCs, the procedure of replacing BIOS contents is sometimes refered to as:</t>
-  </si>
-  <si>
     <t>Direct memory access DMA</t>
   </si>
   <si>
@@ -491,27 +488,15 @@
     <t>A+S</t>
   </si>
   <si>
-    <t>which Microsoft Windows OS utility can be used to view basic information about computers BIOS</t>
-  </si>
-  <si>
     <t>WINVER&gt;EXE</t>
   </si>
   <si>
     <t>MSINFO32.EXE</t>
   </si>
   <si>
-    <t>controle panel</t>
-  </si>
-  <si>
     <t>SERVICES.MSC</t>
   </si>
   <si>
-    <t>power failure during BIOS upgrade can be the cause of irreversible damage to the computer system</t>
-  </si>
-  <si>
-    <t>after normal system shutdown, when the computer is turned off, contents of the memory used to store BIOS setting are:</t>
-  </si>
-  <si>
     <t>Erased</t>
   </si>
   <si>
@@ -527,18 +512,12 @@
     <t>Rettained</t>
   </si>
   <si>
-    <t>which of the acronyms listed below refers to a series of basic hardware diagnostic test performed by the BIOS after the computer is powered on?</t>
-  </si>
-  <si>
     <t>IDE</t>
   </si>
   <si>
     <t>Qos</t>
   </si>
   <si>
-    <t>after completing the initial diagnostics and assigning system resources, the startup Bios program checks for information about secondary storage devices that might contain the OS.  The list of devices and the order in which they should be checked can be found and arranged in th CMOS setu utility, and this option is commonly refered to as:</t>
-  </si>
-  <si>
     <t>boot record</t>
   </si>
   <si>
@@ -554,9 +533,6 @@
     <t>Boot sequence</t>
   </si>
   <si>
-    <t>in order to work, an integrated component such as Network Interface Card(NIC) on a newly assembled computer system may need to be first</t>
-  </si>
-  <si>
     <t>Enabled in Windows Controle Panel</t>
   </si>
   <si>
@@ -584,9 +560,6 @@
     <t xml:space="preserve">Getting the CMOS setup utility and Enabling the virtualization technology setting </t>
   </si>
   <si>
-    <t>the CMOS setup utility can be accessed by pressing:</t>
-  </si>
-  <si>
     <t>Reset button on the front panel of the computer case</t>
   </si>
   <si>
@@ -614,42 +587,15 @@
     <t>Which of the folowing statements is true</t>
   </si>
   <si>
-    <t xml:space="preserve">aborted BIOS update can be resumed by the transaction recovery system </t>
-  </si>
-  <si>
-    <t>a common securtiy measure is to store BIOS on a non-rewriteable memory chip</t>
-  </si>
-  <si>
-    <t>the process of BIOS update can be aborted and resumed at a later time</t>
-  </si>
-  <si>
     <t>Aborted BIOS update could render the computer unusable</t>
   </si>
   <si>
     <t>aborted BIOS update could render the computer unusable</t>
   </si>
   <si>
-    <t>which type of password provides the hightst level of permissions in BIOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">root </t>
-  </si>
-  <si>
     <t>supervisor</t>
   </si>
   <si>
-    <t>administrator</t>
-  </si>
-  <si>
-    <t>power user</t>
-  </si>
-  <si>
-    <t>what is LoJack?</t>
-  </si>
-  <si>
-    <t>loopback adapter</t>
-  </si>
-  <si>
     <t xml:space="preserve">Secutity feature used for locating stolen desktops, laptops, or tablets </t>
   </si>
   <si>
@@ -662,9 +608,6 @@
     <t xml:space="preserve">Security feature used for locating stolen Desktops, laptops, or tablets </t>
   </si>
   <si>
-    <t>which of the folowing terms refer to a tech that allows for storing passwords, certificates, or encryption keys in a hardware chip?</t>
-  </si>
-  <si>
     <t>Access Controle List (ACL)</t>
   </si>
   <si>
@@ -680,9 +623,6 @@
     <t>Trusted Platform Module(TPM)</t>
   </si>
   <si>
-    <t>while tryign to enable the entire drive encryption feature in windows technician receives the followling error message: "A compatible Trusted Platform Module(TPM) security Device must be present on this computer, but a TPM was not found." knowing that the system had a TPM chip installed, which of the folowing steps might help in solving this problem?</t>
-  </si>
-  <si>
     <t>Re-install OS</t>
   </si>
   <si>
@@ -731,12 +671,6 @@
     <t>Similarly to magnetic drives, Solid State-Drives (SSD) require periodic defragmentation in order to improve system performance.</t>
   </si>
   <si>
-    <t>a tiny sopt on the LCD monitor display screen that permanetly remains black when it should be activated and displaying color is commonly refered to as stuck pixel.</t>
-  </si>
-  <si>
-    <t>a permanent computer display screen discoloration caused by displaying the same static image for extended periods of time is known as:</t>
-  </si>
-  <si>
     <t>Artifact</t>
   </si>
   <si>
@@ -749,9 +683,6 @@
     <t>Dead pixel</t>
   </si>
   <si>
-    <t>which of the folowing command-line utilities allows to test the reachability of a host across an IP network</t>
-  </si>
-  <si>
     <t>NETSTAT</t>
   </si>
   <si>
@@ -770,9 +701,6 @@
     <t>IFCONFIG</t>
   </si>
   <si>
-    <t xml:space="preserve">which of the folowing command-line prompt tools listed below allows to display IP addresses, subnet mask, and default gateway for all adaptors? </t>
-  </si>
-  <si>
     <t>A Linux comand-line utility used for displaying and modifying network interface configuration settings is called</t>
   </si>
   <si>
@@ -791,9 +719,6 @@
     <t>N+</t>
   </si>
   <si>
-    <t>which of the folowing is an example of active eavesdropping</t>
-  </si>
-  <si>
     <t>Phishing</t>
   </si>
   <si>
@@ -845,21 +770,9 @@
     <t>Packed software</t>
   </si>
   <si>
-    <t>well known vulberability</t>
-  </si>
-  <si>
     <t>Vulnerability that is present in already released software but unknown to the software developer</t>
   </si>
   <si>
-    <t>one of the measures for securing network devices includes the practice of disabling unsused ports.</t>
-  </si>
-  <si>
-    <t>a hacker has captured network traffic with cleartext commands sent from the client to the server console. Which of the following ports is being used by the network admin for the client-server communication?</t>
-  </si>
-  <si>
-    <t>which of the folowing answers refers to preferred replacement for SLIP protocol</t>
-  </si>
-  <si>
     <t>PPP</t>
   </si>
   <si>
@@ -875,9 +788,6 @@
     <t>FTPS is an extension to the Secure Shell Protocol (SSH) and runs by default on port number 22</t>
   </si>
   <si>
-    <t>which of the following protocols does not provide authentication?</t>
-  </si>
-  <si>
     <t>FTP</t>
   </si>
   <si>
@@ -890,12 +800,6 @@
     <t>SFTP</t>
   </si>
   <si>
-    <t>of the three exsiting versions of the Simple Network Management Protocol (SNMP) versions 1 and 2 (SNMPv1 and SNMPv2) offer authentication based on community strings sent in an unencrypted form (in cleartext). SNMPv3 provides packet encryption, authentication, and hasning mechanisms that allow for checking whether data has changed in transit.</t>
-  </si>
-  <si>
-    <t>which of the following answers refers to a cryptographic network protocol for secure data communication, remote command-line login, remote command execution, and other secure network services between computers?</t>
-  </si>
-  <si>
     <t>Telnet</t>
   </si>
   <si>
@@ -905,15 +809,9 @@
     <t>Bcrypt</t>
   </si>
   <si>
-    <t>which of the protocols listed below was designed as a secure replacement for Telnet</t>
-  </si>
-  <si>
     <t>LDAP</t>
   </si>
   <si>
-    <t>the SCP protocol is used for:</t>
-  </si>
-  <si>
     <t>Directory access</t>
   </si>
   <si>
@@ -941,9 +839,6 @@
     <t>Default</t>
   </si>
   <si>
-    <t>which of the following solutions provides a shielded environment that protects against unintentional signal leakage and eavesdropping</t>
-  </si>
-  <si>
     <t>SCADA</t>
   </si>
   <si>
@@ -968,9 +863,6 @@
     <t>signature files</t>
   </si>
   <si>
-    <t>the term "DHCP snooping" refers to an exploit that enables operation of a rouge DHCP server on a network.</t>
-  </si>
-  <si>
     <t>Simple Mail Transfer Protocol(SMTP) operates with the use of TCP port:</t>
   </si>
   <si>
@@ -980,9 +872,6 @@
     <t>Port number 5061 is typically used for Session Initiation Protocol (SIP) traffic encrypted with Transport Layre Security (TLS)</t>
   </si>
   <si>
-    <t>port number 5004 is used by:</t>
-  </si>
-  <si>
     <t>MGCP</t>
   </si>
   <si>
@@ -1046,9 +935,6 @@
     <t>Merberos</t>
   </si>
   <si>
-    <t>which of the file transfer protocols listed below runs on port number 69 and does not provide authentication?</t>
-  </si>
-  <si>
     <t>TCP port 445 is used by:</t>
   </si>
   <si>
@@ -1115,9 +1001,6 @@
     <t>Which of the following answers lists the binary notation of the decimal number 192?</t>
   </si>
   <si>
-    <t>an Ipv 4 address consists of:</t>
-  </si>
-  <si>
     <t>32bits</t>
   </si>
   <si>
@@ -1229,9 +1112,6 @@
     <t>S+</t>
   </si>
   <si>
-    <t>a device designed to forward data packets between networks is caled:</t>
-  </si>
-  <si>
     <t>Layer 2 switch</t>
   </si>
   <si>
@@ -1256,9 +1136,6 @@
     <t>Entry</t>
   </si>
   <si>
-    <t xml:space="preserve">a network device designed for managing the optimal distribution of workloads across multiple computing resources is called </t>
-  </si>
-  <si>
     <t>Load balancer</t>
   </si>
   <si>
@@ -1271,9 +1148,6 @@
     <t>Load Balancer</t>
   </si>
   <si>
-    <t>the last default rule on a firewall on a firewall is to deny all traffic.</t>
-  </si>
-  <si>
     <t>A computer network service that allows clients to make indirect network connections to other network services is called:</t>
   </si>
   <si>
@@ -1424,9 +1298,6 @@
     <t>VLAN tagging</t>
   </si>
   <si>
-    <t>wireless networking</t>
-  </si>
-  <si>
     <t>An access control model in which access to resources is granted or denied depending on Access Control List (ACL) entries is also known as:</t>
   </si>
   <si>
@@ -1695,9 +1566,6 @@
   </si>
   <si>
     <t>What is the purpose of non-repudiation?</t>
-  </si>
-  <si>
-    <t>taking hashes ensures that data retains its:</t>
   </si>
   <si>
     <t>Confidentiality</t>
@@ -1974,8 +1842,14 @@
     <t>Remote authentication Dial in user service (RADIUS)</t>
   </si>
   <si>
+    <t xml:space="preserve">TRUE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FALSE </t>
+  </si>
+  <si>
     <r>
-      <t>the main functionality of the basic input/output system (</t>
+      <t>The main functionality of the basic input/output system (</t>
     </r>
     <r>
       <rPr>
@@ -2000,7 +1874,139 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">TRUE </t>
+    <t>In modern PCs, the procedure of replacing BIOS contents is sometimes refered to as:</t>
+  </si>
+  <si>
+    <t>Which Microsoft Windows OS utility can be used to view basic information about computers BIOS</t>
+  </si>
+  <si>
+    <t>Power failure during BIOS upgrade can be the cause of irreversible damage to the computer system</t>
+  </si>
+  <si>
+    <t>After normal system shutdown, when the computer is turned off, contents of the memory used to store BIOS setting are:</t>
+  </si>
+  <si>
+    <t>Which of the acronyms listed below refers to a series of basic hardware diagnostic test performed by the BIOS after the computer is powered on?</t>
+  </si>
+  <si>
+    <t>After completing the initial diagnostics and assigning system resources, the startup Bios program checks for information about secondary storage devices that might contain the OS.  The list of devices and the order In which they should be checked can be found and arranged in th CMOS setu utility, and this option is commonly refered to as:</t>
+  </si>
+  <si>
+    <t>In order to work, an integrated component such as Network Interface Card(NIC) on a newly assembled computer system may need to be first</t>
+  </si>
+  <si>
+    <t>The CMOS setup utility can be accessed by pressing:</t>
+  </si>
+  <si>
+    <t>Which type of password provides the hightst level of permissions in BIOS</t>
+  </si>
+  <si>
+    <t>What is LoJack?</t>
+  </si>
+  <si>
+    <t>Which of the folowing terms refer to a tech that allows for storing passwords, certificates, or encryption keys in a hardware chip?</t>
+  </si>
+  <si>
+    <t>While tryign to enable the entire drive encryption feature in windows technician receives the followling error message: "A compatible Trusted Platform Module(TPM) security Device must be present on this computer, but a TPM was not found." knowing that the system had a TPM chip installed, which of the folowing steps might help in solving this problem?</t>
+  </si>
+  <si>
+    <t>A tiny sopt on the LCD monitor display screen that permanetly remains black when it should be activated and displaying color is commonly refered to as stuck pixel.</t>
+  </si>
+  <si>
+    <t>A permanent computer display screen discoloration caused by displaying the same static image for extended periods of time is known as:</t>
+  </si>
+  <si>
+    <t>Which of the folowing command-line utilities allows to test the reachability of a host across an IP network</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which of the folowing command-line prompt tools listed below allows to display IP addresses, subnet mask, and default gateway for all adaptors? </t>
+  </si>
+  <si>
+    <t>Which of the folowing is an example of active eavesdropping</t>
+  </si>
+  <si>
+    <t>One of the measures for securing network devices includes the practice of disabling unsused ports.</t>
+  </si>
+  <si>
+    <t>Which of the folowing answers refers to preferred replacement for SLIP protocol</t>
+  </si>
+  <si>
+    <t>Which of the following protocols does not provide authentication?</t>
+  </si>
+  <si>
+    <t>Of the three exsiting versions of the Simple Network Management Protocol (SNMP) versions 1 and 2 (SNMPv1 and SNMPv2) offer authentication based on community strings sent in an unencrypted form (in cleartext). SNMPv3 provides packet encryption, authentication, and hasning mechanisms that allow for checking whether data has changed in transit.</t>
+  </si>
+  <si>
+    <t>Which of the following answers refers to a cryptographic network protocol for secure data communication, remote command-line login, remote command execution, and other secure network services between computers?</t>
+  </si>
+  <si>
+    <t>Which of the protocols listed below was designed as a secure replacement for Telnet</t>
+  </si>
+  <si>
+    <t>The SCP protocol is used for:</t>
+  </si>
+  <si>
+    <t>Which of the following solutions provides a shielded environment that protects against unintentional signal leakage and eavesdropping</t>
+  </si>
+  <si>
+    <t>The term "DHCP snooping" refers to an exploit that enables operation of a rouge DHCP server on a network.</t>
+  </si>
+  <si>
+    <t>Port number 5004 is used by:</t>
+  </si>
+  <si>
+    <t>Which of the file transfer protocols listed below runs on port number 69 and does not provide authentication?</t>
+  </si>
+  <si>
+    <t>An Ipv 4 address consists of:</t>
+  </si>
+  <si>
+    <t>A device designed to forward data packets between networks is caled:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A network device designed for managing the optimal distribution of workloads across multiple computing resources is called </t>
+  </si>
+  <si>
+    <t>The last default rule on a firewall on a firewall is to deny all traffic.</t>
+  </si>
+  <si>
+    <t>Taking hashes ensures that data retains its:</t>
+  </si>
+  <si>
+    <t>Well known vulberability</t>
+  </si>
+  <si>
+    <t>Wireless networking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Root </t>
+  </si>
+  <si>
+    <t>Supervisor</t>
+  </si>
+  <si>
+    <t>Administrator</t>
+  </si>
+  <si>
+    <t>Power user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aborted BIOS update can be resumed by the transaction recovery system </t>
+  </si>
+  <si>
+    <t>Loopback adapter</t>
+  </si>
+  <si>
+    <t>A common securtiy measure is to store BIOS on a non-rewriteable memory chip</t>
+  </si>
+  <si>
+    <t>The process of BIOS update can be aborted and resumed at a later time</t>
+  </si>
+  <si>
+    <t>The key set by the motherboard manufacturer for accessing CMOS setup utility during boot</t>
+  </si>
+  <si>
+    <t>Controle panel</t>
   </si>
 </sst>
 </file>
@@ -2379,7 +2385,7 @@
   <dimension ref="A1:H157"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3044,138 +3050,138 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>649</v>
+        <v>607</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>650</v>
-      </c>
-      <c r="C26" s="1" t="b">
-        <v>0</v>
+        <v>605</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>606</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="1" t="b">
-        <v>1</v>
+      <c r="F26" s="1" t="s">
+        <v>605</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>576</v>
+        <v>532</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>647</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>646</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="F27" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="D28" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>159</v>
-      </c>
       <c r="F28" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>578</v>
+        <v>534</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>160</v>
+        <v>610</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>650</v>
-      </c>
-      <c r="C29" s="1" t="b">
-        <v>0</v>
+        <v>605</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>606</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="1" t="b">
-        <v>1</v>
+      <c r="F29" s="1" t="s">
+        <v>605</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>576</v>
+        <v>532</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>166</v>
-      </c>
       <c r="G30" s="1" t="s">
-        <v>579</v>
+        <v>535</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>167</v>
+        <v>612</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>11</v>
@@ -3184,625 +3190,625 @@
         <v>11</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>580</v>
+        <v>536</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>170</v>
+        <v>613</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>581</v>
+        <v>537</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>176</v>
+        <v>614</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>645</v>
+        <v>601</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>644</v>
+        <v>600</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>186</v>
+        <v>615</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>188</v>
+        <v>651</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>582</v>
+        <v>538</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>196</v>
+        <v>647</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>197</v>
+        <v>649</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>198</v>
+        <v>650</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>583</v>
+        <v>539</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>201</v>
+        <v>616</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>202</v>
+        <v>643</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>203</v>
+        <v>644</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>204</v>
+        <v>645</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>205</v>
+        <v>646</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>584</v>
+        <v>540</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>206</v>
+        <v>617</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>207</v>
+        <v>648</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>585</v>
+        <v>541</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>212</v>
+        <v>618</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>213</v>
+        <v>194</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>216</v>
+        <v>197</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>586</v>
+        <v>542</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>218</v>
+        <v>619</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>219</v>
+        <v>199</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="G41" s="1"/>
       <c r="H41" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>587</v>
+        <v>543</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>588</v>
+        <v>544</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>650</v>
-      </c>
-      <c r="C44" s="1" t="b">
-        <v>0</v>
+        <v>605</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>606</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
-      <c r="F44" s="1" t="b">
-        <v>0</v>
+      <c r="F44" s="1" t="s">
+        <v>606</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>235</v>
+        <v>620</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>650</v>
-      </c>
-      <c r="C45" s="1" t="b">
-        <v>0</v>
+        <v>605</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>606</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
-      <c r="F45" s="1" t="b">
-        <v>0</v>
+      <c r="F45" s="1" t="s">
+        <v>606</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>236</v>
+        <v>621</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>237</v>
+        <v>215</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>238</v>
+        <v>216</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>239</v>
+        <v>217</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>240</v>
+        <v>218</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>239</v>
+        <v>217</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>589</v>
+        <v>545</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>241</v>
+        <v>622</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>242</v>
+        <v>219</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>244</v>
+        <v>221</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>245</v>
+        <v>222</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>245</v>
+        <v>222</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>590</v>
+        <v>546</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>248</v>
+        <v>623</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>242</v>
+        <v>219</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>247</v>
+        <v>224</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>244</v>
+        <v>221</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>591</v>
+        <v>547</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>249</v>
+        <v>225</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>247</v>
+        <v>224</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>246</v>
+        <v>223</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>247</v>
+        <v>224</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>592</v>
+        <v>548</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>244</v>
+        <v>221</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>252</v>
+        <v>228</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>242</v>
+        <v>219</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>244</v>
+        <v>221</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>593</v>
+        <v>549</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>255</v>
+        <v>624</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>256</v>
+        <v>231</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>257</v>
+        <v>232</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>258</v>
+        <v>233</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>259</v>
+        <v>234</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>259</v>
+        <v>234</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>594</v>
+        <v>550</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>260</v>
+        <v>235</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>261</v>
+        <v>236</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>262</v>
+        <v>237</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>263</v>
+        <v>238</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>264</v>
+        <v>239</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>262</v>
+        <v>237</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>595</v>
+        <v>551</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>265</v>
+        <v>240</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>266</v>
+        <v>241</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>267</v>
+        <v>242</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>268</v>
+        <v>243</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>269</v>
+        <v>244</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>266</v>
+        <v>241</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>596</v>
+        <v>552</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>270</v>
+        <v>245</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>271</v>
+        <v>246</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>272</v>
+        <v>247</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>273</v>
+        <v>641</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>274</v>
+        <v>248</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>274</v>
+        <v>248</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>275</v>
+        <v>625</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>650</v>
-      </c>
-      <c r="C55" s="1" t="b">
-        <v>0</v>
+        <v>605</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>606</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
-      <c r="F55" s="1" t="b">
-        <v>1</v>
+      <c r="F55" s="1" t="s">
+        <v>605</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="B56" s="1">
         <v>49</v>
@@ -3820,289 +3826,289 @@
         <v>23</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>277</v>
+        <v>626</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>278</v>
+        <v>249</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>279</v>
+        <v>250</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>280</v>
+        <v>251</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>281</v>
+        <v>252</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>278</v>
+        <v>249</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>597</v>
+        <v>553</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>282</v>
+        <v>253</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>650</v>
-      </c>
-      <c r="C58" s="1" t="b">
-        <v>0</v>
+        <v>605</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>606</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
-      <c r="F58" s="1" t="b">
-        <v>1</v>
+      <c r="F58" s="1" t="s">
+        <v>605</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>283</v>
+        <v>627</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>284</v>
+        <v>254</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>285</v>
+        <v>255</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>286</v>
+        <v>256</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>287</v>
+        <v>257</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>286</v>
+        <v>256</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>598</v>
+        <v>554</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>288</v>
+        <v>628</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>650</v>
-      </c>
-      <c r="C60" s="1" t="b">
-        <v>0</v>
+        <v>605</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>606</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
-      <c r="F60" s="1" t="b">
-        <v>1</v>
+      <c r="F60" s="1" t="s">
+        <v>605</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>289</v>
+        <v>629</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>290</v>
+        <v>258</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>291</v>
+        <v>259</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>292</v>
+        <v>260</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>286</v>
+        <v>256</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>291</v>
+        <v>259</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>599</v>
+        <v>555</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>293</v>
+        <v>630</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>291</v>
+        <v>259</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>294</v>
+        <v>261</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>284</v>
+        <v>254</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>280</v>
+        <v>251</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>291</v>
+        <v>259</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>599</v>
+        <v>555</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>295</v>
+        <v>631</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>296</v>
+        <v>262</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>297</v>
+        <v>263</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>298</v>
+        <v>264</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>299</v>
+        <v>265</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>297</v>
+        <v>263</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>300</v>
+        <v>266</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>301</v>
+        <v>267</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>302</v>
+        <v>268</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>303</v>
+        <v>269</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>304</v>
+        <v>270</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>301</v>
+        <v>267</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>305</v>
+        <v>632</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>307</v>
+        <v>272</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>306</v>
+        <v>271</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>308</v>
+        <v>273</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>309</v>
+        <v>274</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>307</v>
+        <v>272</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>310</v>
+        <v>275</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>311</v>
+        <v>276</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>643</v>
+        <v>599</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>642</v>
+        <v>598</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>312</v>
+        <v>277</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>313</v>
+        <v>278</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>314</v>
+        <v>633</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>650</v>
-      </c>
-      <c r="C67" s="1" t="b">
-        <v>0</v>
+        <v>605</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>606</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
-      <c r="F67" s="1" t="b">
-        <v>0</v>
+      <c r="F67" s="1" t="s">
+        <v>606</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>315</v>
+        <v>279</v>
       </c>
       <c r="B68" s="1">
         <v>110</v>
@@ -4120,15 +4126,15 @@
         <v>25</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>316</v>
+        <v>280</v>
       </c>
       <c r="B69" s="1">
         <v>5004</v>
@@ -4146,63 +4152,63 @@
         <v>5060</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>317</v>
+        <v>281</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>650</v>
-      </c>
-      <c r="C70" s="1" t="b">
-        <v>0</v>
+        <v>605</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>606</v>
       </c>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
-      <c r="F70" s="1" t="b">
-        <v>0</v>
+      <c r="F70" s="1" t="s">
+        <v>606</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>318</v>
+        <v>634</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>319</v>
+        <v>282</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>320</v>
+        <v>283</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>321</v>
+        <v>284</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>322</v>
+        <v>285</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>320</v>
+        <v>283</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>323</v>
+        <v>286</v>
       </c>
       <c r="B72" s="1">
         <v>5004</v>
@@ -4220,111 +4226,111 @@
         <v>5005</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>324</v>
+        <v>287</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>319</v>
+        <v>282</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>321</v>
+        <v>284</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>325</v>
+        <v>288</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>320</v>
+        <v>283</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>321</v>
+        <v>284</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>326</v>
+        <v>289</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>650</v>
-      </c>
-      <c r="C74" s="1" t="b">
-        <v>0</v>
+        <v>605</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>606</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
-      <c r="F74" s="1" t="b">
-        <v>0</v>
+      <c r="F74" s="1" t="s">
+        <v>606</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>327</v>
+        <v>290</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>650</v>
-      </c>
-      <c r="C75" s="1" t="b">
-        <v>0</v>
+        <v>605</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>606</v>
       </c>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
-      <c r="F75" s="1" t="b">
-        <v>0</v>
+      <c r="F75" s="1" t="s">
+        <v>606</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>328</v>
+        <v>291</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>320</v>
+        <v>283</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>329</v>
+        <v>292</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>330</v>
+        <v>293</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>322</v>
+        <v>285</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>330</v>
+        <v>293</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>331</v>
+        <v>294</v>
       </c>
       <c r="B77" s="1">
         <v>161</v>
@@ -4342,41 +4348,41 @@
         <v>161</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>332</v>
+        <v>295</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>290</v>
+        <v>258</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>291</v>
+        <v>259</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>292</v>
+        <v>260</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>286</v>
+        <v>256</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>291</v>
+        <v>259</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>599</v>
+        <v>555</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>333</v>
+        <v>296</v>
       </c>
       <c r="B79" s="1">
         <v>49</v>
@@ -4394,15 +4400,15 @@
         <v>23</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>334</v>
+        <v>297</v>
       </c>
       <c r="B80" s="1">
         <v>20</v>
@@ -4420,15 +4426,15 @@
         <v>22</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>335</v>
+        <v>298</v>
       </c>
       <c r="B81" s="1">
         <v>139</v>
@@ -4446,93 +4452,93 @@
         <v>53</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>336</v>
+        <v>299</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>337</v>
+        <v>300</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>648</v>
+        <v>604</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>338</v>
+        <v>301</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>339</v>
+        <v>302</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>337</v>
+        <v>300</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>600</v>
+        <v>556</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>340</v>
+        <v>635</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>284</v>
+        <v>254</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>286</v>
+        <v>256</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>285</v>
+        <v>255</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>287</v>
+        <v>257</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>286</v>
+        <v>256</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>598</v>
+        <v>554</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>341</v>
+        <v>303</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>342</v>
+        <v>304</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>343</v>
+        <v>305</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>344</v>
+        <v>306</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>320</v>
+        <v>283</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>343</v>
+        <v>305</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>601</v>
+        <v>557</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>345</v>
+        <v>307</v>
       </c>
       <c r="B85" s="1">
         <v>1701</v>
@@ -4550,115 +4556,115 @@
         <v>3389</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>346</v>
+        <v>308</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>650</v>
-      </c>
-      <c r="C86" s="1" t="b">
-        <v>0</v>
+        <v>605</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>606</v>
       </c>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
-      <c r="F86" s="1" t="b">
-        <v>1</v>
+      <c r="F86" s="1" t="s">
+        <v>605</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>347</v>
+        <v>309</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>348</v>
+        <v>310</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>349</v>
+        <v>311</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>349</v>
+        <v>311</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>350</v>
+        <v>312</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>350</v>
+        <v>312</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>351</v>
+        <v>313</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>352</v>
+        <v>314</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>353</v>
+        <v>315</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>354</v>
+        <v>316</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>355</v>
+        <v>317</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>352</v>
+        <v>314</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>356</v>
+        <v>318</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>357</v>
+        <v>319</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>358</v>
+        <v>320</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>359</v>
+        <v>321</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>360</v>
+        <v>322</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>361</v>
+        <v>323</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>602</v>
+        <v>558</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>362</v>
+        <v>324</v>
       </c>
       <c r="B90" s="1">
         <v>10101100</v>
@@ -4676,41 +4682,41 @@
         <v>11000000</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>363</v>
+        <v>636</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>364</v>
+        <v>325</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>365</v>
+        <v>326</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>366</v>
+        <v>327</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>367</v>
+        <v>328</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>364</v>
+        <v>325</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>362</v>
+        <v>324</v>
       </c>
       <c r="B92" s="1">
         <v>168</v>
@@ -4728,142 +4734,142 @@
         <v>172</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>368</v>
+        <v>329</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>369</v>
+        <v>330</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>371</v>
+        <v>332</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>372</v>
+        <v>333</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>370</v>
+        <v>331</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>370</v>
+        <v>331</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>373</v>
+        <v>334</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>377</v>
+        <v>338</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>378</v>
+        <v>339</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>379</v>
+        <v>340</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>380</v>
+        <v>341</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>377</v>
+        <v>338</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>373</v>
+        <v>334</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>374</v>
+        <v>335</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>381</v>
+        <v>342</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>375</v>
+        <v>336</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>376</v>
+        <v>337</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>375</v>
+        <v>336</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>382</v>
+        <v>343</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>650</v>
-      </c>
-      <c r="C96" s="1" t="b">
-        <v>0</v>
+        <v>605</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>606</v>
       </c>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
-      <c r="F96" s="1" t="b">
-        <v>1</v>
+      <c r="F96" s="1" t="s">
+        <v>605</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>383</v>
+        <v>344</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>384</v>
+        <v>345</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>385</v>
+        <v>346</v>
       </c>
       <c r="D97" s="1"/>
       <c r="E97" s="1" t="s">
-        <v>386</v>
+        <v>347</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>385</v>
+        <v>346</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>387</v>
+        <v>348</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>330</v>
+        <v>293</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>46</v>
@@ -4878,1338 +4884,1338 @@
         <v>45</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>603</v>
+        <v>559</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>388</v>
+        <v>349</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>389</v>
+        <v>350</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>390</v>
+        <v>351</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>390</v>
+        <v>351</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>391</v>
+        <v>352</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>389</v>
+        <v>350</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>604</v>
+        <v>560</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>392</v>
+        <v>353</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>389</v>
+        <v>350</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>390</v>
+        <v>351</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>393</v>
+        <v>354</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>391</v>
+        <v>352</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>394</v>
+        <v>355</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>605</v>
+        <v>561</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>395</v>
+        <v>356</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>396</v>
+        <v>357</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>397</v>
+        <v>358</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>398</v>
+        <v>359</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>399</v>
+        <v>360</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>397</v>
+        <v>358</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>606</v>
+        <v>562</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>401</v>
+        <v>637</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>402</v>
+        <v>362</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>403</v>
+        <v>363</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>404</v>
+        <v>364</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>405</v>
+        <v>365</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>405</v>
+        <v>365</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>607</v>
+        <v>563</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>406</v>
+        <v>366</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>301</v>
+        <v>267</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>407</v>
+        <v>367</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>408</v>
+        <v>368</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>409</v>
+        <v>369</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>407</v>
+        <v>367</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>410</v>
+        <v>638</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>411</v>
+        <v>370</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>412</v>
+        <v>371</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>397</v>
+        <v>358</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>413</v>
+        <v>372</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>414</v>
+        <v>373</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>608</v>
+        <v>564</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>415</v>
+        <v>639</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>650</v>
-      </c>
-      <c r="C105" s="1" t="b">
-        <v>0</v>
+        <v>605</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>606</v>
       </c>
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
-      <c r="F105" s="1" t="b">
-        <v>1</v>
+      <c r="F105" s="1" t="s">
+        <v>605</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>416</v>
+        <v>374</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>417</v>
+        <v>375</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>418</v>
+        <v>376</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>419</v>
+        <v>377</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>420</v>
+        <v>378</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>418</v>
+        <v>376</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>609</v>
+        <v>565</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>421</v>
+        <v>379</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>422</v>
+        <v>380</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>404</v>
+        <v>364</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>397</v>
+        <v>358</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>412</v>
+        <v>371</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>412</v>
+        <v>371</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>610</v>
+        <v>566</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>423</v>
+        <v>381</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>650</v>
-      </c>
-      <c r="C108" s="1" t="b">
-        <v>0</v>
+        <v>605</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>606</v>
       </c>
       <c r="D108" s="1"/>
       <c r="E108" s="1"/>
-      <c r="F108" s="1" t="b">
-        <v>1</v>
+      <c r="F108" s="1" t="s">
+        <v>605</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>424</v>
+        <v>382</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>425</v>
+        <v>383</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>426</v>
+        <v>384</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>427</v>
+        <v>385</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>428</v>
+        <v>386</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>425</v>
+        <v>383</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>611</v>
+        <v>567</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>429</v>
+        <v>387</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>430</v>
+        <v>388</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>431</v>
+        <v>389</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>432</v>
+        <v>390</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>433</v>
+        <v>391</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>431</v>
+        <v>389</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>612</v>
+        <v>568</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>434</v>
+        <v>392</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>435</v>
+        <v>393</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>436</v>
+        <v>394</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>437</v>
+        <v>395</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>438</v>
+        <v>396</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>435</v>
+        <v>393</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>613</v>
+        <v>569</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>439</v>
+        <v>397</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>440</v>
+        <v>398</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>441</v>
+        <v>399</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>442</v>
+        <v>400</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>443</v>
+        <v>401</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>442</v>
+        <v>400</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>614</v>
+        <v>570</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>444</v>
+        <v>402</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>445</v>
+        <v>403</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>446</v>
+        <v>404</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>447</v>
+        <v>405</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>448</v>
+        <v>406</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>446</v>
+        <v>404</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>615</v>
+        <v>571</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>449</v>
+        <v>407</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>422</v>
+        <v>380</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>412</v>
+        <v>371</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>450</v>
+        <v>408</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>451</v>
+        <v>409</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>422</v>
+        <v>380</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>616</v>
+        <v>572</v>
       </c>
       <c r="H114" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>452</v>
+        <v>410</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>453</v>
+        <v>411</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>454</v>
+        <v>412</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>455</v>
+        <v>413</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>456</v>
+        <v>414</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>456</v>
+        <v>414</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>617</v>
+        <v>573</v>
       </c>
       <c r="H115" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>457</v>
+        <v>415</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>458</v>
+        <v>416</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>459</v>
+        <v>417</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>460</v>
+        <v>418</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>461</v>
+        <v>419</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>460</v>
+        <v>418</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>618</v>
+        <v>574</v>
       </c>
       <c r="H116" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>462</v>
+        <v>420</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>463</v>
+        <v>421</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>464</v>
+        <v>422</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>465</v>
+        <v>423</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>466</v>
+        <v>642</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>464</v>
+        <v>422</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>619</v>
+        <v>575</v>
       </c>
       <c r="H117" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>467</v>
+        <v>424</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>468</v>
+        <v>425</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>469</v>
+        <v>426</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>470</v>
+        <v>427</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>471</v>
+        <v>428</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>471</v>
+        <v>428</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>620</v>
+        <v>576</v>
       </c>
       <c r="H118" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>472</v>
+        <v>429</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>473</v>
+        <v>430</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>413</v>
+        <v>372</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>474</v>
+        <v>431</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>397</v>
+        <v>358</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>475</v>
+        <v>432</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>621</v>
+        <v>577</v>
       </c>
       <c r="H119" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>476</v>
+        <v>433</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>477</v>
+        <v>434</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>478</v>
+        <v>435</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>441</v>
+        <v>399</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>479</v>
+        <v>436</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>441</v>
+        <v>399</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>622</v>
+        <v>578</v>
       </c>
       <c r="H120" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>480</v>
+        <v>437</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>650</v>
-      </c>
-      <c r="C121" s="1" t="b">
-        <v>0</v>
+        <v>605</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>606</v>
       </c>
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
-      <c r="F121" s="1" t="b">
-        <v>1</v>
+      <c r="F121" s="1" t="s">
+        <v>605</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>481</v>
+        <v>438</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>482</v>
+        <v>439</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>483</v>
+        <v>440</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>484</v>
+        <v>441</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>485</v>
+        <v>442</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>483</v>
+        <v>440</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>623</v>
+        <v>579</v>
       </c>
       <c r="H122" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>486</v>
+        <v>443</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>650</v>
-      </c>
-      <c r="C123" s="1" t="b">
-        <v>0</v>
+        <v>605</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>606</v>
       </c>
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
-      <c r="F123" s="1" t="b">
-        <v>0</v>
+      <c r="F123" s="1" t="s">
+        <v>606</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H123" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>487</v>
+        <v>444</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>488</v>
+        <v>445</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>489</v>
+        <v>446</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>490</v>
+        <v>447</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>491</v>
+        <v>448</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>492</v>
+        <v>449</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H124" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>493</v>
+        <v>450</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>494</v>
+        <v>451</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>495</v>
+        <v>452</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>496</v>
+        <v>453</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>497</v>
+        <v>454</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>498</v>
+        <v>455</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H125" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>499</v>
+        <v>456</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>267</v>
+        <v>242</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>268</v>
+        <v>243</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>500</v>
+        <v>457</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>266</v>
+        <v>241</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>399</v>
+        <v>360</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>624</v>
+        <v>580</v>
       </c>
       <c r="H126" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>501</v>
+        <v>458</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>502</v>
+        <v>459</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>503</v>
+        <v>460</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>504</v>
+        <v>461</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>505</v>
+        <v>462</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>504</v>
+        <v>461</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H127" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>506</v>
+        <v>463</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>267</v>
+        <v>242</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>507</v>
+        <v>464</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>500</v>
+        <v>457</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>508</v>
+        <v>465</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>507</v>
+        <v>464</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>625</v>
+        <v>581</v>
       </c>
       <c r="H128" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>509</v>
+        <v>466</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>510</v>
+        <v>467</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>267</v>
+        <v>242</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>511</v>
+        <v>468</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>268</v>
+        <v>243</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>268</v>
+        <v>243</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>626</v>
+        <v>582</v>
       </c>
       <c r="H129" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>512</v>
+        <v>469</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>513</v>
+        <v>470</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>268</v>
+        <v>243</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>510</v>
+        <v>467</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>267</v>
+        <v>242</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>513</v>
+        <v>470</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>627</v>
+        <v>583</v>
       </c>
       <c r="H130" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>514</v>
+        <v>471</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>515</v>
+        <v>472</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>267</v>
+        <v>242</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>516</v>
+        <v>473</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>517</v>
+        <v>474</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>516</v>
+        <v>473</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>628</v>
+        <v>584</v>
       </c>
       <c r="H131" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>518</v>
+        <v>475</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>519</v>
+        <v>476</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>520</v>
+        <v>477</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>521</v>
+        <v>478</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>522</v>
+        <v>479</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>520</v>
+        <v>477</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H132" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>523</v>
+        <v>480</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>420</v>
+        <v>378</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>524</v>
+        <v>481</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>525</v>
+        <v>482</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>526</v>
+        <v>483</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>525</v>
+        <v>482</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>629</v>
+        <v>585</v>
       </c>
       <c r="H133" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>527</v>
+        <v>484</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>528</v>
+        <v>485</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>525</v>
+        <v>482</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>513</v>
+        <v>470</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>420</v>
+        <v>378</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>420</v>
+        <v>378</v>
       </c>
       <c r="G134" s="1" t="s">
-        <v>630</v>
+        <v>586</v>
       </c>
       <c r="H134" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>529</v>
+        <v>486</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>510</v>
+        <v>467</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>530</v>
+        <v>487</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>513</v>
+        <v>470</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>531</v>
+        <v>488</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>510</v>
+        <v>467</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>631</v>
+        <v>587</v>
       </c>
       <c r="H135" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>532</v>
+        <v>489</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>533</v>
+        <v>490</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>524</v>
+        <v>481</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>534</v>
+        <v>491</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>535</v>
+        <v>492</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>524</v>
+        <v>481</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>524</v>
+        <v>481</v>
       </c>
       <c r="H136" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>536</v>
+        <v>493</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>516</v>
+        <v>473</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>267</v>
+        <v>242</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>515</v>
+        <v>472</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>268</v>
+        <v>243</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>515</v>
+        <v>472</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>632</v>
+        <v>588</v>
       </c>
       <c r="H137" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>537</v>
+        <v>494</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>538</v>
+        <v>495</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>539</v>
+        <v>496</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>540</v>
+        <v>497</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>541</v>
+        <v>498</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>539</v>
+        <v>496</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>633</v>
+        <v>589</v>
       </c>
       <c r="H138" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>542</v>
+        <v>499</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>531</v>
+        <v>488</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>525</v>
+        <v>482</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>543</v>
+        <v>500</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>420</v>
+        <v>378</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>531</v>
+        <v>488</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>634</v>
+        <v>590</v>
       </c>
       <c r="H139" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>544</v>
+        <v>501</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>256</v>
+        <v>231</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>257</v>
+        <v>232</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>258</v>
+        <v>233</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>259</v>
+        <v>234</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>259</v>
+        <v>234</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>635</v>
+        <v>591</v>
       </c>
       <c r="H140" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>545</v>
+        <v>502</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>650</v>
-      </c>
-      <c r="C141" s="1" t="b">
-        <v>0</v>
+        <v>605</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>606</v>
       </c>
       <c r="D141" s="1"/>
       <c r="E141" s="1"/>
-      <c r="F141" s="1" t="b">
-        <v>1</v>
+      <c r="F141" s="1" t="s">
+        <v>605</v>
       </c>
       <c r="G141" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H141" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>546</v>
+        <v>503</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>541</v>
+        <v>498</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>547</v>
+        <v>504</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>420</v>
+        <v>378</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>548</v>
+        <v>505</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>541</v>
+        <v>498</v>
       </c>
       <c r="G142" s="1" t="s">
-        <v>636</v>
+        <v>592</v>
       </c>
       <c r="H142" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>549</v>
+        <v>506</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>301</v>
+        <v>267</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>550</v>
+        <v>507</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>302</v>
+        <v>268</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>303</v>
+        <v>269</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>301</v>
+        <v>267</v>
       </c>
       <c r="G143" s="1" t="s">
-        <v>637</v>
+        <v>593</v>
       </c>
       <c r="H143" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>551</v>
+        <v>508</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>552</v>
+        <v>509</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>553</v>
+        <v>510</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>554</v>
+        <v>511</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>555</v>
+        <v>512</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>554</v>
+        <v>511</v>
       </c>
       <c r="G144" s="1" t="s">
-        <v>638</v>
+        <v>594</v>
       </c>
       <c r="H144" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>556</v>
+        <v>513</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>494</v>
+        <v>451</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>495</v>
+        <v>452</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>496</v>
+        <v>453</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>497</v>
+        <v>454</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>498</v>
+        <v>455</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H145" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>557</v>
+        <v>640</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>558</v>
+        <v>514</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>559</v>
+        <v>515</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>560</v>
+        <v>516</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>561</v>
+        <v>517</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>562</v>
+        <v>518</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>639</v>
+        <v>595</v>
       </c>
       <c r="H146" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>563</v>
+        <v>519</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>564</v>
+        <v>520</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>565</v>
+        <v>521</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>566</v>
+        <v>522</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>567</v>
+        <v>523</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>565</v>
+        <v>521</v>
       </c>
       <c r="G147" s="1" t="s">
-        <v>640</v>
+        <v>596</v>
       </c>
       <c r="H147" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>568</v>
+        <v>524</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>488</v>
+        <v>445</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>489</v>
+        <v>446</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>490</v>
+        <v>447</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>491</v>
+        <v>448</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>490</v>
+        <v>447</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H148" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>569</v>
+        <v>525</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>650</v>
-      </c>
-      <c r="C149" s="1" t="b">
-        <v>0</v>
+        <v>605</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>606</v>
       </c>
       <c r="D149" s="1"/>
       <c r="E149" s="1"/>
-      <c r="F149" s="1" t="b">
-        <v>1</v>
+      <c r="F149" s="1" t="s">
+        <v>605</v>
       </c>
       <c r="G149" s="1" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="H149" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>570</v>
+        <v>526</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>571</v>
+        <v>527</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>572</v>
+        <v>528</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>573</v>
+        <v>529</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>574</v>
+        <v>530</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>573</v>
+        <v>529</v>
       </c>
       <c r="G150" s="1" t="s">
-        <v>641</v>
+        <v>597</v>
       </c>
       <c r="H150" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>